<commit_message>
Uploading newest EPS US files
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7076F41-4AE3-4F66-8436-DA24B6EE8FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8CC1E9-0943-416B-8E2D-F1243AAEE080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="758">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2300,6 +2300,12 @@
   </si>
   <si>
     <t>Dispatch Priority by Electricity Source</t>
+  </si>
+  <si>
+    <t>PVTStL</t>
+  </si>
+  <si>
+    <t>Policy Vehicle Types Subject to LCFS</t>
   </si>
 </sst>
 </file>
@@ -3121,11 +3127,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G271"/>
+  <dimension ref="A1:G272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99:XFD99"/>
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A250" sqref="A250:F250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6979,35 +6985,35 @@
         <v>100</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>443</v>
+        <v>756</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F250" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G250" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+        <v>757</v>
+      </c>
+      <c r="F250" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>644</v>
+        <v>443</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="F251" s="5" t="s">
-        <v>101</v>
+        <v>444</v>
+      </c>
+      <c r="F251" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G251" s="2" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -7015,10 +7021,10 @@
         <v>73</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>507</v>
+        <v>644</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>508</v>
+        <v>645</v>
       </c>
       <c r="F252" s="5" t="s">
         <v>101</v>
@@ -7029,13 +7035,13 @@
         <v>73</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>245</v>
+        <v>507</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F253" s="14" t="s">
-        <v>258</v>
+        <v>508</v>
+      </c>
+      <c r="F253" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -7043,13 +7049,13 @@
         <v>73</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>298</v>
+        <v>245</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F254" s="5" t="s">
-        <v>101</v>
+        <v>246</v>
+      </c>
+      <c r="F254" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -7057,13 +7063,13 @@
         <v>73</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>646</v>
+        <v>298</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="F255" s="4" t="s">
-        <v>100</v>
+        <v>297</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -7071,13 +7077,13 @@
         <v>73</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>234</v>
+        <v>646</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F256" s="5" t="s">
-        <v>101</v>
+        <v>647</v>
+      </c>
+      <c r="F256" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -7085,10 +7091,10 @@
         <v>73</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>630</v>
+        <v>234</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>631</v>
+        <v>235</v>
       </c>
       <c r="F257" s="5" t="s">
         <v>101</v>
@@ -7099,13 +7105,13 @@
         <v>73</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>226</v>
+        <v>630</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F258" s="12" t="s">
-        <v>250</v>
+        <v>631</v>
+      </c>
+      <c r="F258" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
@@ -7113,13 +7119,13 @@
         <v>73</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>524</v>
+        <v>226</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F259" s="14" t="s">
-        <v>258</v>
+        <v>227</v>
+      </c>
+      <c r="F259" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -7127,16 +7133,13 @@
         <v>73</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E260" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F260" s="5" t="s">
-        <v>101</v>
+        <v>525</v>
+      </c>
+      <c r="F260" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -7144,44 +7147,44 @@
         <v>73</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>224</v>
+        <v>522</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>225</v>
+        <v>523</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="F261" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>648</v>
+        <v>224</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="F262" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="263" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="F262" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>585</v>
+        <v>648</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="F263" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G263" s="2" t="s">
-        <v>588</v>
+        <v>649</v>
+      </c>
+      <c r="F263" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="264" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7189,98 +7192,101 @@
         <v>73</v>
       </c>
       <c r="B264" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F264" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G264" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B265" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="C265" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F264" s="16" t="s">
+      <c r="F265" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G264" s="2" t="s">
+      <c r="G265" s="2" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="17" t="s">
+    <row r="266" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B265" s="17" t="s">
+      <c r="B266" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="C265" s="17" t="s">
+      <c r="C266" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="D265" s="17"/>
-      <c r="E265" s="17"/>
-      <c r="F265" s="20" t="s">
+      <c r="D266" s="17"/>
+      <c r="E266" s="17"/>
+      <c r="F266" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G265" s="17"/>
-    </row>
-    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D266" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F266" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G266" s="17"/>
+    </row>
+    <row r="267" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>222</v>
+        <v>91</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>221</v>
+        <v>92</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>403</v>
+        <v>315</v>
       </c>
       <c r="F267" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>249</v>
+        <v>403</v>
       </c>
       <c r="F268" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>351</v>
+        <v>247</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F269" s="4" t="s">
-        <v>100</v>
+        <v>248</v>
+      </c>
+      <c r="D269" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F269" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -7288,36 +7294,50 @@
         <v>90</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>565</v>
+        <v>351</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D270" s="2" t="s">
-        <v>567</v>
+        <v>352</v>
       </c>
       <c r="F270" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="17" t="s">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B271" s="17" t="s">
+      <c r="B271" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F271" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B272" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="C271" s="17" t="s">
+      <c r="C272" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D271" s="17" t="s">
+      <c r="D272" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="E271" s="17"/>
-      <c r="F271" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G271" s="17"/>
+      <c r="E272" s="17"/>
+      <c r="F272" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G272" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update with newest US model
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8CC1E9-0943-416B-8E2D-F1243AAEE080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8129B8F3-CD5F-469F-8564-550C965CF605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="761">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2239,12 +2239,6 @@
     <t>BAU Heat Rates, BAU Start Year Capacities</t>
   </si>
   <si>
-    <t>BRACP</t>
-  </si>
-  <si>
-    <t>BAU RPS Alternative Compliance Payment</t>
-  </si>
-  <si>
     <t>Annual CapEx per Unit Capacity, BAU Construction Cost per Unit Capacity, Annual Fixed O&amp;M Cost per Unit Capacity, Variable O&amp;M Cost per Unit Elec Output, BAU Soft Costs per Unit Capacity, Annual CapEx per Unit Capacity, Spur Line Construction Cost per Unit Capacity, BAU CCS Retrofit Costs per Unit Capacity</t>
   </si>
   <si>
@@ -2306,6 +2300,21 @@
   </si>
   <si>
     <t>Policy Vehicle Types Subject to LCFS</t>
+  </si>
+  <si>
+    <t>FY</t>
+  </si>
+  <si>
+    <t>Future Year</t>
+  </si>
+  <si>
+    <t>If you change Initial Time, you need to update this file</t>
+  </si>
+  <si>
+    <t>RACP</t>
+  </si>
+  <si>
+    <t>RPS Alternative Compliance Payment</t>
   </si>
 </sst>
 </file>
@@ -3127,11 +3136,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G272"/>
+  <dimension ref="A1:G273"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A250" sqref="A250:F250"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4062,50 +4071,52 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="17" t="s">
+    <row r="59" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C59" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="E59" s="17"/>
       <c r="F59" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="G59" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>99</v>
-      </c>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>759</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>760</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G60" s="17"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>202</v>
+        <v>41</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>99</v>
@@ -4116,13 +4127,13 @@
         <v>38</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>100</v>
+        <v>202</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -4130,49 +4141,46 @@
         <v>38</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>546</v>
+        <v>40</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>547</v>
+        <v>42</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C65" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="21" t="s">
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G65" s="17" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4180,61 +4188,61 @@
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>181</v>
+        <v>658</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>732</v>
+        <v>659</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>733</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>660</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>328</v>
+        <v>181</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>732</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>604</v>
+        <v>328</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>687</v>
+        <v>604</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>689</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>100</v>
+        <v>603</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4242,33 +4250,33 @@
         <v>43</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>175</v>
+        <v>687</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>595</v>
+        <v>175</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="F71" s="12" t="s">
-        <v>250</v>
+        <v>174</v>
+      </c>
+      <c r="F71" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4276,58 +4284,61 @@
         <v>43</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>44</v>
+        <v>595</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F73" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>696</v>
+        <v>45</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>735</v>
+        <v>696</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>101</v>
+        <v>697</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4403,7 +4414,7 @@
         <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>101</v>
@@ -4414,10 +4425,10 @@
         <v>43</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>101</v>
@@ -4445,13 +4456,13 @@
         <v>43</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>740</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>742</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>101</v>
@@ -4504,10 +4515,10 @@
         <v>43</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F87" s="4" t="s">
         <v>100</v>
@@ -4558,7 +4569,7 @@
         <v>664</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>101</v>
@@ -4617,10 +4628,10 @@
         <v>43</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>101</v>
@@ -4679,10 +4690,10 @@
         <v>43</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>100</v>
@@ -4800,7 +4811,7 @@
         <v>673</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F106" s="14" t="s">
         <v>258</v>
@@ -5022,13 +5033,13 @@
         <v>43</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="D121" s="2" t="s">
         <v>749</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>751</v>
       </c>
       <c r="F121" s="3" t="s">
         <v>99</v>
@@ -6382,37 +6393,40 @@
         <v>548</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="17" t="s">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B209" s="17" t="s">
+      <c r="B209" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="F209" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B210" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C209" s="17" t="s">
+      <c r="C210" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D209" s="17"/>
-      <c r="E209" s="17"/>
-      <c r="F209" s="22" t="s">
+      <c r="D210" s="17"/>
+      <c r="E210" s="17"/>
+      <c r="F210" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="G209" s="17" t="s">
+      <c r="G210" s="17" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="F210" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6420,13 +6434,13 @@
         <v>73</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>551</v>
+        <v>635</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>101</v>
+        <v>636</v>
+      </c>
+      <c r="F211" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6434,13 +6448,13 @@
         <v>73</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>74</v>
+        <v>551</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F212" s="4" t="s">
-        <v>100</v>
+        <v>552</v>
+      </c>
+      <c r="F212" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6448,41 +6462,41 @@
         <v>73</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F213" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F213" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>555</v>
+        <v>75</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>556</v>
+        <v>83</v>
       </c>
       <c r="F214" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>411</v>
+        <v>555</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="F215" s="4" t="s">
-        <v>100</v>
+        <v>556</v>
+      </c>
+      <c r="F215" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6490,10 +6504,10 @@
         <v>73</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>680</v>
+        <v>411</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>681</v>
+        <v>412</v>
       </c>
       <c r="F216" s="4" t="s">
         <v>100</v>
@@ -6504,13 +6518,13 @@
         <v>73</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>553</v>
+        <v>680</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="F217" s="5" t="s">
-        <v>101</v>
+        <v>681</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -6518,24 +6532,24 @@
         <v>73</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>283</v>
+        <v>553</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F218" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="219" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+      <c r="F218" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>99</v>
@@ -6546,27 +6560,27 @@
         <v>73</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E220" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F220" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F220" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>621</v>
+        <v>236</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>622</v>
+        <v>237</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="F221" s="5" t="s">
         <v>101</v>
@@ -6577,10 +6591,10 @@
         <v>73</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F222" s="5" t="s">
         <v>101</v>
@@ -6591,10 +6605,10 @@
         <v>73</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>232</v>
+        <v>623</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>233</v>
+        <v>624</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>101</v>
@@ -6605,10 +6619,10 @@
         <v>73</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>101</v>
@@ -6619,13 +6633,10 @@
         <v>73</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>637</v>
+        <v>228</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="D225" s="2" t="s">
-        <v>639</v>
+        <v>229</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>101</v>
@@ -6636,10 +6647,13 @@
         <v>73</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>625</v>
+        <v>637</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>626</v>
+        <v>638</v>
+      </c>
+      <c r="D226" s="2" t="s">
+        <v>639</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>101</v>
@@ -6650,13 +6664,13 @@
         <v>73</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>718</v>
+        <v>625</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="F227" s="3" t="s">
-        <v>99</v>
+        <v>626</v>
+      </c>
+      <c r="F227" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -6664,10 +6678,10 @@
         <v>73</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>640</v>
+        <v>718</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>641</v>
+        <v>719</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>99</v>
@@ -6678,10 +6692,10 @@
         <v>73</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>612</v>
+        <v>640</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>613</v>
+        <v>641</v>
       </c>
       <c r="F229" s="3" t="s">
         <v>99</v>
@@ -6692,13 +6706,13 @@
         <v>73</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="F230" s="4" t="s">
-        <v>100</v>
+        <v>613</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -6706,44 +6720,44 @@
         <v>73</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>241</v>
+        <v>590</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>242</v>
+        <v>591</v>
       </c>
       <c r="F231" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F232" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G232" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="F232" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>76</v>
+        <v>285</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F233" s="5" t="s">
-        <v>101</v>
+        <v>286</v>
+      </c>
+      <c r="F233" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G233" s="2" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6751,10 +6765,10 @@
         <v>73</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F234" s="5" t="s">
         <v>101</v>
@@ -6765,10 +6779,10 @@
         <v>73</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F235" s="5" t="s">
         <v>101</v>
@@ -6779,44 +6793,44 @@
         <v>73</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F236" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="237" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="F236" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>627</v>
+        <v>79</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="F237" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="F237" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>448</v>
+        <v>627</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="F238" s="4" t="s">
-        <v>100</v>
+        <v>628</v>
+      </c>
+      <c r="D238" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="F238" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -6824,41 +6838,41 @@
         <v>73</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>478</v>
+        <v>448</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>479</v>
+        <v>449</v>
       </c>
       <c r="F239" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>642</v>
+        <v>478</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="F240" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+      <c r="F240" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>752</v>
+        <v>642</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="F241" s="3" t="s">
-        <v>99</v>
+        <v>643</v>
+      </c>
+      <c r="F241" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -6866,10 +6880,10 @@
         <v>73</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>80</v>
+        <v>750</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>88</v>
+        <v>751</v>
       </c>
       <c r="F242" s="3" t="s">
         <v>99</v>
@@ -6880,30 +6894,27 @@
         <v>73</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>549</v>
+        <v>80</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="F243" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>293</v>
+        <v>549</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F244" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G244" s="2" t="s">
-        <v>335</v>
+        <v>550</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="245" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6911,10 +6922,10 @@
         <v>73</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F245" s="16" t="s">
         <v>303</v>
@@ -6928,10 +6939,10 @@
         <v>73</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>239</v>
+        <v>295</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
       <c r="F246" s="16" t="s">
         <v>303</v>
@@ -6940,35 +6951,38 @@
         <v>335</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E247" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F247" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="F247" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G247" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>698</v>
+        <v>230</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>699</v>
-      </c>
-      <c r="F248" s="5" t="s">
-        <v>238</v>
+        <v>231</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F248" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="249" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6976,58 +6990,58 @@
         <v>73</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>81</v>
+        <v>698</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F249" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+        <v>699</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>756</v>
+        <v>81</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>757</v>
+        <v>89</v>
       </c>
       <c r="F250" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>443</v>
+        <v>754</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F251" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G251" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+        <v>755</v>
+      </c>
+      <c r="F251" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>644</v>
+        <v>443</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="F252" s="5" t="s">
-        <v>101</v>
+        <v>444</v>
+      </c>
+      <c r="F252" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G252" s="2" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -7035,10 +7049,10 @@
         <v>73</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>507</v>
+        <v>644</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>508</v>
+        <v>645</v>
       </c>
       <c r="F253" s="5" t="s">
         <v>101</v>
@@ -7049,13 +7063,13 @@
         <v>73</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>245</v>
+        <v>507</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F254" s="14" t="s">
-        <v>258</v>
+        <v>508</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -7063,13 +7077,13 @@
         <v>73</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>298</v>
+        <v>245</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F255" s="5" t="s">
-        <v>101</v>
+        <v>246</v>
+      </c>
+      <c r="F255" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -7077,13 +7091,13 @@
         <v>73</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>646</v>
+        <v>298</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="F256" s="4" t="s">
-        <v>100</v>
+        <v>297</v>
+      </c>
+      <c r="F256" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -7091,13 +7105,13 @@
         <v>73</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>234</v>
+        <v>646</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F257" s="5" t="s">
-        <v>101</v>
+        <v>647</v>
+      </c>
+      <c r="F257" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -7105,10 +7119,10 @@
         <v>73</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>630</v>
+        <v>234</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>631</v>
+        <v>235</v>
       </c>
       <c r="F258" s="5" t="s">
         <v>101</v>
@@ -7119,13 +7133,13 @@
         <v>73</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>226</v>
+        <v>630</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F259" s="12" t="s">
-        <v>250</v>
+        <v>631</v>
+      </c>
+      <c r="F259" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -7133,13 +7147,13 @@
         <v>73</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>524</v>
+        <v>226</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F260" s="14" t="s">
-        <v>258</v>
+        <v>227</v>
+      </c>
+      <c r="F260" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -7147,16 +7161,13 @@
         <v>73</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E261" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F261" s="5" t="s">
-        <v>101</v>
+        <v>525</v>
+      </c>
+      <c r="F261" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -7164,44 +7175,44 @@
         <v>73</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>224</v>
+        <v>522</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>225</v>
+        <v>523</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="F262" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>648</v>
+        <v>224</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="F263" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="264" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="F263" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>585</v>
+        <v>648</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="F264" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G264" s="2" t="s">
-        <v>588</v>
+        <v>649</v>
+      </c>
+      <c r="F264" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="265" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7209,98 +7220,101 @@
         <v>73</v>
       </c>
       <c r="B265" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F265" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G265" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B266" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="C266" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F265" s="16" t="s">
+      <c r="F266" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G265" s="2" t="s">
+      <c r="G266" s="2" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A266" s="17" t="s">
+    <row r="267" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A267" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B266" s="17" t="s">
+      <c r="B267" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="C266" s="17" t="s">
+      <c r="C267" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="D266" s="17"/>
-      <c r="E266" s="17"/>
-      <c r="F266" s="20" t="s">
+      <c r="D267" s="17"/>
+      <c r="E267" s="17"/>
+      <c r="F267" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G266" s="17"/>
-    </row>
-    <row r="267" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A267" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D267" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F267" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G267" s="17"/>
+    </row>
+    <row r="268" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>222</v>
+        <v>91</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>221</v>
+        <v>92</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>403</v>
+        <v>315</v>
       </c>
       <c r="F268" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>249</v>
+        <v>403</v>
       </c>
       <c r="F269" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>351</v>
+        <v>247</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F270" s="4" t="s">
-        <v>100</v>
+        <v>248</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F270" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -7308,36 +7322,50 @@
         <v>90</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>565</v>
+        <v>351</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D271" s="2" t="s">
-        <v>567</v>
+        <v>352</v>
       </c>
       <c r="F271" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="17" t="s">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B272" s="17" t="s">
+      <c r="B272" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F272" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A273" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B273" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="C272" s="17" t="s">
+      <c r="C273" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D272" s="17" t="s">
+      <c r="D273" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="E272" s="17"/>
-      <c r="F272" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G272" s="17"/>
+      <c r="E273" s="17"/>
+      <c r="F273" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G273" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update to latest 4.0
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8129B8F3-CD5F-469F-8564-550C965CF605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F78FFEB-53F7-446A-A303-A6DFABECBEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7875" yWindow="4455" windowWidth="37485" windowHeight="17055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="759">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2102,12 +2102,6 @@
   </si>
   <si>
     <t>Fraction of EVs Used for Grid Balancing on Average Day, Fraction of EV Battery Capacity Used for Grid Balancing when EV is Used for Grid Balancing</t>
-  </si>
-  <si>
-    <t>DATAiRC</t>
-  </si>
-  <si>
-    <t>Demand-Altering Technology Assistance in RPS Compliance</t>
   </si>
   <si>
     <t>CCSTaSC</t>
@@ -3136,11 +3130,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G273"/>
+  <dimension ref="A1:G272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A84" sqref="A84:XFD84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,10 +3303,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>99</v>
@@ -3702,13 +3696,13 @@
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>704</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>705</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>706</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>101</v>
@@ -3719,10 +3713,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>100</v>
@@ -3739,7 +3733,7 @@
         <v>417</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>101</v>
@@ -3756,7 +3750,7 @@
         <v>410</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>101</v>
@@ -3767,10 +3761,10 @@
         <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>101</v>
@@ -3781,10 +3775,10 @@
         <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>100</v>
@@ -3798,7 +3792,7 @@
         <v>575</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>100</v>
@@ -3853,7 +3847,7 @@
         <v>142</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3946,16 +3940,16 @@
         <v>413</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>180</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4082,7 +4076,7 @@
         <v>465</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>180</v>
@@ -4096,10 +4090,10 @@
         <v>413</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
@@ -4208,10 +4202,10 @@
         <v>181</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>100</v>
@@ -4290,7 +4284,7 @@
         <v>596</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>250</v>
@@ -4332,10 +4326,10 @@
         <v>43</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>99</v>
@@ -4366,10 +4360,10 @@
         <v>43</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>99</v>
@@ -4414,7 +4408,7 @@
         <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>101</v>
@@ -4425,10 +4419,10 @@
         <v>43</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>101</v>
@@ -4456,13 +4450,13 @@
         <v>43</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>738</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>739</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>740</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>101</v>
@@ -4473,27 +4467,27 @@
         <v>43</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>690</v>
+        <v>650</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>650</v>
+        <v>309</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>101</v>
+        <v>310</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4501,27 +4495,30 @@
         <v>43</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>309</v>
+        <v>750</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>310</v>
+        <v>751</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>752</v>
+        <v>47</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>100</v>
+        <v>171</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4529,16 +4526,16 @@
         <v>43</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>47</v>
+        <v>288</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>713</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>99</v>
+        <v>290</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4546,16 +4543,16 @@
         <v>43</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>288</v>
+        <v>663</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>289</v>
+        <v>664</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>100</v>
+        <v>739</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4563,154 +4560,151 @@
         <v>43</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>663</v>
+        <v>169</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>664</v>
+        <v>170</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>169</v>
+        <v>674</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>170</v>
+        <v>675</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>674</v>
+        <v>608</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>608</v>
+        <v>740</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>609</v>
+        <v>741</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>742</v>
+        <v>489</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>489</v>
+        <v>177</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>177</v>
+        <v>721</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>723</v>
+        <v>742</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>724</v>
+        <v>743</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>744</v>
+        <v>593</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>745</v>
+        <v>594</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>593</v>
+        <v>606</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>100</v>
+        <v>607</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4718,13 +4712,13 @@
         <v>43</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>99</v>
+        <v>598</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4732,10 +4726,10 @@
         <v>43</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>597</v>
+        <v>665</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>598</v>
+        <v>666</v>
       </c>
       <c r="F101" s="4" t="s">
         <v>100</v>
@@ -4746,13 +4740,13 @@
         <v>43</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>665</v>
+        <v>48</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="F102" s="4" t="s">
-        <v>100</v>
+        <v>53</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4760,72 +4754,72 @@
         <v>43</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>196</v>
+        <v>49</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>49</v>
+        <v>672</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="F105" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>672</v>
+        <v>186</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="F106" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>186</v>
+        <v>580</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>187</v>
+        <v>581</v>
       </c>
       <c r="F107" s="4" t="s">
         <v>100</v>
@@ -4836,109 +4830,109 @@
         <v>43</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>580</v>
+        <v>203</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>203</v>
+        <v>684</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>204</v>
+        <v>685</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>205</v>
+        <v>686</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>684</v>
+        <v>601</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>685</v>
+        <v>602</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B111" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="F111" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="F111" s="3" t="s">
+      <c r="B112" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B112" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="F112" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>700</v>
+        <v>452</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>701</v>
+        <v>453</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>702</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>452</v>
+        <v>682</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>100</v>
+        <v>683</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4946,13 +4940,13 @@
         <v>43</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>682</v>
+        <v>654</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="F115" s="14" t="s">
-        <v>258</v>
+        <v>655</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4960,10 +4954,10 @@
         <v>43</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="F116" s="4" t="s">
         <v>100</v>
@@ -4974,27 +4968,27 @@
         <v>43</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>656</v>
+        <v>575</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>657</v>
+        <v>576</v>
       </c>
       <c r="F117" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>575</v>
+        <v>652</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="F118" s="4" t="s">
-        <v>100</v>
+        <v>653</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -5002,27 +4996,30 @@
         <v>43</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>652</v>
+        <v>599</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>653</v>
+        <v>600</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>597</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>599</v>
+        <v>745</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>597</v>
+        <v>746</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>747</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>99</v>
@@ -5033,51 +5030,51 @@
         <v>43</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>747</v>
+        <v>714</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="F122" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B123" s="17" t="s">
+      <c r="B122" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="C123" s="17" t="s">
+      <c r="C122" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="D123" s="17" t="s">
+      <c r="D122" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="E123" s="17"/>
-      <c r="F123" s="21" t="s">
+      <c r="E122" s="17"/>
+      <c r="F122" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G123" s="17" t="s">
+      <c r="G122" s="17" t="s">
         <v>350</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5085,117 +5082,117 @@
         <v>275</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>715</v>
+        <v>634</v>
       </c>
       <c r="F124" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>634</v>
+        <v>272</v>
       </c>
       <c r="F125" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>271</v>
+        <v>418</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F126" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>418</v>
+        <v>183</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F128" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
+    <row r="129" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F129" s="4" t="s">
+      <c r="B129" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C129" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="B130" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C130" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="D130" s="17"/>
-      <c r="E130" s="17"/>
-      <c r="F130" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G130" s="17"/>
+      <c r="G129" s="17"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>99</v>
@@ -5206,47 +5203,44 @@
         <v>55</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>473</v>
+        <v>380</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>475</v>
+        <v>381</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>380</v>
+        <v>56</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>381</v>
+        <v>59</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>56</v>
+        <v>313</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>99</v>
+        <v>314</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -5254,10 +5248,13 @@
         <v>55</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>313</v>
+        <v>526</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>314</v>
+        <v>527</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>528</v>
       </c>
       <c r="F135" s="5" t="s">
         <v>101</v>
@@ -5268,16 +5265,13 @@
         <v>55</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>526</v>
+        <v>544</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="F136" s="5" t="s">
-        <v>101</v>
+        <v>545</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -5285,58 +5279,61 @@
         <v>55</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>544</v>
+        <v>610</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+        <v>611</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>610</v>
+        <v>57</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="F138" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>57</v>
+        <v>311</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F139" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>311</v>
+        <v>390</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F140" s="5" t="s">
-        <v>101</v>
+        <v>393</v>
+      </c>
+      <c r="F140" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5344,16 +5341,16 @@
         <v>55</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F141" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5361,131 +5358,128 @@
         <v>55</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F142" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>392</v>
+        <v>58</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="F143" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G143" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>58</v>
+        <v>376</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>61</v>
+        <v>340</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F144" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="F144" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F145" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>388</v>
+        <v>441</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="F146" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="24" t="s">
+        <v>404</v>
+      </c>
+      <c r="B147" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="C147" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="D147" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="E147" s="24"/>
+      <c r="F147" s="19" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="F147" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G147" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="24" t="s">
-        <v>404</v>
-      </c>
-      <c r="B148" s="24" t="s">
-        <v>406</v>
-      </c>
-      <c r="C148" s="24" t="s">
-        <v>407</v>
-      </c>
-      <c r="D148" s="24" t="s">
-        <v>408</v>
-      </c>
-      <c r="E148" s="24"/>
-      <c r="F148" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G148" s="24"/>
+      <c r="G147" s="24"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="F149" s="5" t="s">
-        <v>101</v>
+        <v>367</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -5493,24 +5487,27 @@
         <v>357</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F150" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="F151" s="4" t="s">
         <v>100</v>
@@ -5521,95 +5518,95 @@
         <v>357</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="F153" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F154" s="6" t="s">
         <v>142</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B155" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F155" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G155" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="B156" s="17" t="s">
+      <c r="B155" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="C156" s="17" t="s">
+      <c r="C155" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="D156" s="17"/>
-      <c r="E156" s="17"/>
-      <c r="F156" s="20" t="s">
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G156" s="17"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G155" s="17"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F156" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>206</v>
+        <v>519</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F157" s="12" t="s">
-        <v>250</v>
+        <v>520</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="F157" s="14" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5617,16 +5614,16 @@
         <v>63</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>519</v>
+        <v>667</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>520</v>
+        <v>668</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="F158" s="14" t="s">
-        <v>400</v>
+        <v>669</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5634,16 +5631,19 @@
         <v>63</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>667</v>
+        <v>197</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="F159" s="4" t="s">
-        <v>100</v>
+        <v>198</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F159" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G159" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5651,19 +5651,13 @@
         <v>63</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>197</v>
+        <v>326</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F160" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G160" s="2" t="s">
-        <v>339</v>
+        <v>327</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5671,27 +5665,27 @@
         <v>63</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>326</v>
+        <v>64</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F161" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>64</v>
+        <v>497</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F162" s="4" t="s">
-        <v>100</v>
+        <v>498</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -5699,13 +5693,16 @@
         <v>63</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>497</v>
+        <v>65</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="F163" s="5" t="s">
-        <v>101</v>
+        <v>68</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5713,61 +5710,61 @@
         <v>63</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>65</v>
+        <v>563</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F164" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G164" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+      <c r="F164" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>563</v>
+        <v>516</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="F165" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+      <c r="F165" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G165" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>516</v>
+        <v>199</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="F166" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G166" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="F166" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>199</v>
+        <v>66</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F167" s="4" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F167" s="14" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5775,16 +5772,13 @@
         <v>63</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>66</v>
+        <v>190</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F168" s="14" t="s">
-        <v>400</v>
+        <v>191</v>
+      </c>
+      <c r="F168" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5792,13 +5786,13 @@
         <v>63</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>190</v>
+        <v>277</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F169" s="4" t="s">
-        <v>100</v>
+        <v>280</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5806,10 +5800,10 @@
         <v>63</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F170" s="5" t="s">
         <v>101</v>
@@ -5820,13 +5814,13 @@
         <v>63</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F171" s="5" t="s">
-        <v>101</v>
+        <v>282</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5834,13 +5828,13 @@
         <v>63</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>279</v>
+        <v>568</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F172" s="4" t="s">
-        <v>100</v>
+        <v>569</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5848,13 +5842,13 @@
         <v>63</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>568</v>
+        <v>477</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="F173" s="5" t="s">
-        <v>101</v>
+        <v>476</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5862,58 +5856,61 @@
         <v>63</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>477</v>
+        <v>493</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>476</v>
+        <v>494</v>
       </c>
       <c r="F174" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
+    <row r="175" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="F175" s="4" t="s">
+      <c r="B175" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="C175" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B176" s="17" t="s">
-        <v>495</v>
-      </c>
-      <c r="C176" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="D176" s="17"/>
-      <c r="E176" s="17"/>
-      <c r="F176" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G176" s="17"/>
-    </row>
-    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G175" s="17"/>
+    </row>
+    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>560</v>
+        <v>719</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>561</v>
+        <v>720</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>562</v>
+        <v>718</v>
       </c>
       <c r="F177" s="3" t="s">
         <v>99</v>
@@ -5924,13 +5921,10 @@
         <v>420</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>721</v>
+        <v>428</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>722</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>720</v>
+        <v>429</v>
       </c>
       <c r="F178" s="3" t="s">
         <v>99</v>
@@ -5941,10 +5935,10 @@
         <v>420</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="F179" s="3" t="s">
         <v>99</v>
@@ -5955,10 +5949,10 @@
         <v>420</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>430</v>
+        <v>401</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>431</v>
+        <v>402</v>
       </c>
       <c r="F180" s="3" t="s">
         <v>99</v>
@@ -5969,44 +5963,44 @@
         <v>420</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>401</v>
+        <v>432</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>402</v>
+        <v>433</v>
       </c>
       <c r="F181" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>432</v>
+        <v>616</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>433</v>
+        <v>618</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="F182" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>616</v>
+        <v>434</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="D183" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>99</v>
@@ -6017,27 +6011,30 @@
         <v>420</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>422</v>
+        <v>531</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="F185" s="3" t="s">
-        <v>99</v>
+        <v>532</v>
+      </c>
+      <c r="F185" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G185" s="2" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6045,65 +6042,62 @@
         <v>420</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>531</v>
+        <v>480</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="F186" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G186" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F186" s="3"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>480</v>
+        <v>529</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="D187" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="F187" s="3"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="F187" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G187" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>529</v>
+        <v>503</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="F188" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G188" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="E189" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="F189" s="3" t="s">
-        <v>99</v>
+        <v>502</v>
+      </c>
+      <c r="F189" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -6111,10 +6105,10 @@
         <v>420</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>502</v>
+        <v>468</v>
       </c>
       <c r="F190" s="5" t="s">
         <v>101</v>
@@ -6125,10 +6119,10 @@
         <v>420</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>467</v>
+        <v>423</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>468</v>
+        <v>425</v>
       </c>
       <c r="F191" s="5" t="s">
         <v>101</v>
@@ -6139,10 +6133,10 @@
         <v>420</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>423</v>
+        <v>469</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>425</v>
+        <v>470</v>
       </c>
       <c r="F192" s="5" t="s">
         <v>101</v>
@@ -6153,106 +6147,106 @@
         <v>420</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>469</v>
+        <v>542</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="F193" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>542</v>
+        <v>426</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="F194" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+      <c r="F194" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G194" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>426</v>
+        <v>570</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="F195" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G195" s="2" t="s">
-        <v>535</v>
+        <v>571</v>
+      </c>
+      <c r="F195" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="2" t="s">
+      <c r="A196" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>571</v>
-      </c>
+      <c r="B196" s="17" t="s">
+        <v>491</v>
+      </c>
+      <c r="C196" s="17" t="s">
+        <v>492</v>
+      </c>
+      <c r="D196" s="17"/>
+      <c r="E196" s="17"/>
       <c r="F196" s="19" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="17" t="s">
-        <v>420</v>
-      </c>
-      <c r="B197" s="17" t="s">
-        <v>491</v>
-      </c>
-      <c r="C197" s="17" t="s">
-        <v>492</v>
-      </c>
-      <c r="D197" s="17"/>
-      <c r="E197" s="17"/>
-      <c r="F197" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G197" s="17"/>
-    </row>
-    <row r="198" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G196" s="17"/>
+    </row>
+    <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F197" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>209</v>
+        <v>304</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F198" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F198" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>304</v>
+        <v>211</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F199" s="12" t="s">
-        <v>250</v>
+        <v>212</v>
+      </c>
+      <c r="F199" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6260,13 +6254,16 @@
         <v>93</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F200" s="5" t="s">
-        <v>101</v>
+        <v>214</v>
+      </c>
+      <c r="F200" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6274,44 +6271,41 @@
         <v>93</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F201" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G201" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="F201" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>215</v>
+        <v>94</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>220</v>
+        <v>97</v>
       </c>
       <c r="F202" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>94</v>
+        <v>216</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F203" s="5" t="s">
-        <v>101</v>
+        <v>217</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6319,114 +6313,114 @@
         <v>93</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F204" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F204" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F205" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B206" s="17" t="s">
+      <c r="B205" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C206" s="17" t="s">
+      <c r="C205" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D206" s="17"/>
-      <c r="E206" s="17"/>
-      <c r="F206" s="20" t="s">
+      <c r="D205" s="17"/>
+      <c r="E205" s="17"/>
+      <c r="F205" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G206" s="17"/>
+      <c r="G205" s="17"/>
+    </row>
+    <row r="206" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F206" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="207" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>71</v>
+        <v>192</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>72</v>
+        <v>194</v>
       </c>
       <c r="F207" s="6" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>192</v>
+        <v>754</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>194</v>
+        <v>755</v>
       </c>
       <c r="F208" s="6" t="s">
         <v>142</v>
       </c>
       <c r="G208" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="F209" s="6" t="s">
+      <c r="B209" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C209" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D209" s="17"/>
+      <c r="E209" s="17"/>
+      <c r="F209" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="G209" s="2" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B210" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C210" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D210" s="17"/>
-      <c r="E210" s="17"/>
-      <c r="F210" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="G210" s="17" t="s">
+      <c r="G209" s="17" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="F210" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -6434,13 +6428,13 @@
         <v>73</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>635</v>
+        <v>551</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="F211" s="4" t="s">
-        <v>100</v>
+        <v>552</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6448,13 +6442,13 @@
         <v>73</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>551</v>
+        <v>74</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="F212" s="5" t="s">
-        <v>101</v>
+        <v>82</v>
+      </c>
+      <c r="F212" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6462,41 +6456,41 @@
         <v>73</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F213" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="F213" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>75</v>
+        <v>555</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>83</v>
+        <v>556</v>
       </c>
       <c r="F214" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>555</v>
+        <v>411</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="F215" s="5" t="s">
-        <v>101</v>
+        <v>412</v>
+      </c>
+      <c r="F215" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6504,10 +6498,10 @@
         <v>73</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>411</v>
+        <v>680</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>412</v>
+        <v>681</v>
       </c>
       <c r="F216" s="4" t="s">
         <v>100</v>
@@ -6518,13 +6512,13 @@
         <v>73</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>680</v>
+        <v>553</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="F217" s="4" t="s">
-        <v>100</v>
+        <v>554</v>
+      </c>
+      <c r="F217" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -6532,24 +6526,24 @@
         <v>73</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>553</v>
+        <v>283</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="F218" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="F218" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>283</v>
+        <v>256</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>284</v>
+        <v>257</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>99</v>
@@ -6560,27 +6554,27 @@
         <v>73</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F220" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F220" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>236</v>
+        <v>621</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E221" s="2" t="s">
-        <v>379</v>
+        <v>622</v>
       </c>
       <c r="F221" s="5" t="s">
         <v>101</v>
@@ -6591,10 +6585,10 @@
         <v>73</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="F222" s="5" t="s">
         <v>101</v>
@@ -6605,10 +6599,10 @@
         <v>73</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>623</v>
+        <v>232</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>624</v>
+        <v>233</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>101</v>
@@ -6619,10 +6613,10 @@
         <v>73</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>101</v>
@@ -6633,10 +6627,13 @@
         <v>73</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>228</v>
+        <v>637</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>229</v>
+        <v>638</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>639</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>101</v>
@@ -6647,13 +6644,10 @@
         <v>73</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="D226" s="2" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>101</v>
@@ -6664,13 +6658,13 @@
         <v>73</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>625</v>
+        <v>716</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="F227" s="5" t="s">
-        <v>101</v>
+        <v>717</v>
+      </c>
+      <c r="F227" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -6678,10 +6672,10 @@
         <v>73</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>718</v>
+        <v>640</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>719</v>
+        <v>641</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>99</v>
@@ -6692,10 +6686,10 @@
         <v>73</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>640</v>
+        <v>612</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>641</v>
+        <v>613</v>
       </c>
       <c r="F229" s="3" t="s">
         <v>99</v>
@@ -6706,13 +6700,13 @@
         <v>73</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>612</v>
+        <v>590</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="F230" s="3" t="s">
-        <v>99</v>
+        <v>591</v>
+      </c>
+      <c r="F230" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -6720,44 +6714,44 @@
         <v>73</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>590</v>
+        <v>241</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>591</v>
+        <v>242</v>
       </c>
       <c r="F231" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>241</v>
+        <v>285</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F232" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="F232" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G232" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>285</v>
+        <v>76</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F233" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G233" s="2" t="s">
-        <v>334</v>
+        <v>84</v>
+      </c>
+      <c r="F233" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6765,10 +6759,10 @@
         <v>73</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F234" s="5" t="s">
         <v>101</v>
@@ -6779,10 +6773,10 @@
         <v>73</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F235" s="5" t="s">
         <v>101</v>
@@ -6793,44 +6787,44 @@
         <v>73</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F236" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="F236" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>79</v>
+        <v>627</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F237" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="238" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="F237" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>627</v>
+        <v>448</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="F238" s="5" t="s">
-        <v>101</v>
+        <v>449</v>
+      </c>
+      <c r="F238" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -6838,41 +6832,41 @@
         <v>73</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>448</v>
+        <v>478</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>449</v>
+        <v>479</v>
       </c>
       <c r="F239" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>478</v>
+        <v>642</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F240" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>643</v>
+      </c>
+      <c r="F240" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>642</v>
+        <v>748</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="F241" s="5" t="s">
-        <v>101</v>
+        <v>749</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -6880,10 +6874,10 @@
         <v>73</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>750</v>
+        <v>80</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>751</v>
+        <v>88</v>
       </c>
       <c r="F242" s="3" t="s">
         <v>99</v>
@@ -6894,27 +6888,30 @@
         <v>73</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>80</v>
+        <v>549</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F243" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>549</v>
+        <v>293</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="F244" s="5" t="s">
-        <v>101</v>
+        <v>294</v>
+      </c>
+      <c r="F244" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G244" s="2" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="245" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6922,10 +6919,10 @@
         <v>73</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F245" s="16" t="s">
         <v>303</v>
@@ -6939,10 +6936,10 @@
         <v>73</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>295</v>
+        <v>239</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>296</v>
+        <v>240</v>
       </c>
       <c r="F246" s="16" t="s">
         <v>303</v>
@@ -6951,38 +6948,35 @@
         <v>335</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="F247" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G247" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F247" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>230</v>
+        <v>696</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E248" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F248" s="4" t="s">
-        <v>100</v>
+        <v>697</v>
+      </c>
+      <c r="F248" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="249" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6990,58 +6984,58 @@
         <v>73</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>698</v>
+        <v>81</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>699</v>
-      </c>
-      <c r="F249" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F249" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>81</v>
+        <v>752</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>89</v>
+        <v>753</v>
       </c>
       <c r="F250" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>754</v>
+        <v>443</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="F251" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+      <c r="F251" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G251" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>443</v>
+        <v>644</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F252" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G252" s="2" t="s">
-        <v>377</v>
+        <v>645</v>
+      </c>
+      <c r="F252" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -7049,10 +7043,10 @@
         <v>73</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>644</v>
+        <v>507</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>645</v>
+        <v>508</v>
       </c>
       <c r="F253" s="5" t="s">
         <v>101</v>
@@ -7063,13 +7057,13 @@
         <v>73</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>507</v>
+        <v>245</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="F254" s="5" t="s">
-        <v>101</v>
+        <v>246</v>
+      </c>
+      <c r="F254" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -7077,13 +7071,13 @@
         <v>73</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F255" s="14" t="s">
-        <v>258</v>
+        <v>297</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -7091,13 +7085,13 @@
         <v>73</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>298</v>
+        <v>646</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F256" s="5" t="s">
-        <v>101</v>
+        <v>647</v>
+      </c>
+      <c r="F256" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -7105,13 +7099,13 @@
         <v>73</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>646</v>
+        <v>234</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="F257" s="4" t="s">
-        <v>100</v>
+        <v>235</v>
+      </c>
+      <c r="F257" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -7119,10 +7113,10 @@
         <v>73</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>234</v>
+        <v>630</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>235</v>
+        <v>631</v>
       </c>
       <c r="F258" s="5" t="s">
         <v>101</v>
@@ -7133,13 +7127,13 @@
         <v>73</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>630</v>
+        <v>226</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="F259" s="5" t="s">
-        <v>101</v>
+        <v>227</v>
+      </c>
+      <c r="F259" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -7147,13 +7141,13 @@
         <v>73</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>226</v>
+        <v>524</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F260" s="12" t="s">
-        <v>250</v>
+        <v>525</v>
+      </c>
+      <c r="F260" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -7161,13 +7155,16 @@
         <v>73</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F261" s="14" t="s">
-        <v>258</v>
+        <v>523</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F261" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -7175,44 +7172,44 @@
         <v>73</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>522</v>
+        <v>224</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E262" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F262" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>224</v>
+        <v>648</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F263" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="264" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>649</v>
+      </c>
+      <c r="F263" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>648</v>
+        <v>585</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="F264" s="20" t="s">
-        <v>100</v>
+        <v>587</v>
+      </c>
+      <c r="F264" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G264" s="2" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="265" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7220,101 +7217,98 @@
         <v>73</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="F265" s="3" t="s">
-        <v>99</v>
+        <v>589</v>
+      </c>
+      <c r="F265" s="16" t="s">
+        <v>303</v>
       </c>
       <c r="G265" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A266" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A266" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B266" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="F266" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G266" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="267" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B267" s="17" t="s">
+      <c r="B266" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="C267" s="17" t="s">
+      <c r="C266" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="D267" s="17"/>
-      <c r="E267" s="17"/>
-      <c r="F267" s="20" t="s">
+      <c r="D266" s="17"/>
+      <c r="E266" s="17"/>
+      <c r="F266" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G267" s="17"/>
-    </row>
-    <row r="268" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G266" s="17"/>
+    </row>
+    <row r="267" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F267" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>91</v>
+        <v>222</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>315</v>
+        <v>403</v>
       </c>
       <c r="F268" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>403</v>
+        <v>249</v>
       </c>
       <c r="F269" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>247</v>
+        <v>351</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D270" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F270" s="5" t="s">
-        <v>101</v>
+        <v>352</v>
+      </c>
+      <c r="F270" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -7322,50 +7316,36 @@
         <v>90</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>351</v>
+        <v>565</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>352</v>
+        <v>566</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>567</v>
       </c>
       <c r="F271" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A272" s="2" t="s">
+    <row r="272" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A272" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B272" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="C272" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="D272" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F272" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="273" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B273" s="17" t="s">
+      <c r="B272" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="C273" s="17" t="s">
+      <c r="C272" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D273" s="17" t="s">
+      <c r="D272" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="E273" s="17"/>
-      <c r="F273" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G273" s="17"/>
+      <c r="E272" s="17"/>
+      <c r="F272" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G272" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update to current eps-us develop
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB7B22F-00E2-4A6E-AEC9-3FB51C71D3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8897B2-1E68-48A6-9A5A-DDB5029AA7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="1660" windowWidth="17280" windowHeight="9670" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="764">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2306,6 +2306,24 @@
   </si>
   <si>
     <t>Max and Min Hourly Electriicty Imports and Exports</t>
+  </si>
+  <si>
+    <t>BPMCRS</t>
+  </si>
+  <si>
+    <t>BAU Policy Mandated Capacity Retrofit Schedule</t>
+  </si>
+  <si>
+    <t>You know particular capacities of particular types of plants will be retrofit with CCUS in particular years (for example, they are already under construction), or you are modeling a region where power plant retrofit decisions are based on government mandates rather than being market-driven</t>
+  </si>
+  <si>
+    <t>PMCRS</t>
+  </si>
+  <si>
+    <t>Policy Mandated Capacity Retrofit Schedule</t>
+  </si>
+  <si>
+    <t>You are modeling a region where power plant CCUS retrofit decisions are based on government mandates rather than being market-driven, and you are setting this policy lever to alter the BAU mandates</t>
   </si>
 </sst>
 </file>
@@ -3127,11 +3145,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G272"/>
+  <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4318,63 +4336,66 @@
         <v>322</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>694</v>
+        <v>758</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>695</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+        <v>759</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>677</v>
+        <v>694</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>203</v>
+        <v>695</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>692</v>
+        <v>677</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>693</v>
+        <v>678</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>160</v>
+        <v>692</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>161</v>
+        <v>693</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>99</v>
@@ -4385,61 +4406,58 @@
         <v>43</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>661</v>
+        <v>160</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>46</v>
+        <v>661</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>730</v>
+        <v>662</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>731</v>
+        <v>46</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>732</v>
+        <v>52</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>730</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>513</v>
+        <v>731</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>515</v>
+        <v>732</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -4447,44 +4465,47 @@
         <v>43</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>733</v>
+        <v>513</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>514</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>650</v>
+        <v>733</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>651</v>
+        <v>734</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>735</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>309</v>
+        <v>650</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>100</v>
+        <v>651</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -4492,64 +4513,61 @@
         <v>43</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>747</v>
+        <v>309</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>748</v>
+        <v>310</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>47</v>
+        <v>747</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+        <v>748</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>288</v>
+        <v>47</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>289</v>
+        <v>171</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>708</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>663</v>
+        <v>288</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>664</v>
+        <v>289</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>101</v>
+        <v>290</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4557,33 +4575,33 @@
         <v>43</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>169</v>
+        <v>663</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>170</v>
+        <v>664</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+        <v>736</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>674</v>
+        <v>169</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>675</v>
+        <v>170</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>100</v>
+        <v>447</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -4591,13 +4609,16 @@
         <v>43</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>608</v>
+        <v>674</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>101</v>
+        <v>675</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -4605,10 +4626,10 @@
         <v>43</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>737</v>
+        <v>608</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>738</v>
+        <v>609</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>101</v>
@@ -4619,89 +4640,89 @@
         <v>43</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>489</v>
+        <v>737</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>738</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>177</v>
+        <v>489</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F95" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>490</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>718</v>
+        <v>177</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>739</v>
+        <v>718</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>740</v>
+        <v>719</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>593</v>
+        <v>739</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>594</v>
+        <v>740</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>99</v>
+        <v>594</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -4709,10 +4730,10 @@
         <v>43</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>756</v>
+        <v>606</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>757</v>
+        <v>607</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>99</v>
@@ -4723,13 +4744,13 @@
         <v>43</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>597</v>
+        <v>756</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>100</v>
+        <v>757</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -4737,10 +4758,10 @@
         <v>43</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>665</v>
+        <v>597</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>666</v>
+        <v>598</v>
       </c>
       <c r="F102" s="4" t="s">
         <v>100</v>
@@ -4751,13 +4772,13 @@
         <v>43</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>48</v>
+        <v>665</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>99</v>
+        <v>666</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -4765,61 +4786,61 @@
         <v>43</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>196</v>
+        <v>48</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>49</v>
+        <v>196</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>672</v>
+        <v>49</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="F106" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>186</v>
+        <v>761</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>100</v>
+        <v>762</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4827,30 +4848,30 @@
         <v>43</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>580</v>
+        <v>672</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>673</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="F108" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>338</v>
+        <v>187</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4858,86 +4879,89 @@
         <v>43</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>684</v>
+        <v>580</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+        <v>581</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>601</v>
+        <v>203</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>602</v>
+        <v>204</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>99</v>
+        <v>205</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B112" s="2" t="s">
-        <v>670</v>
+        <v>684</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="F112" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>685</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>452</v>
+        <v>601</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>453</v>
+        <v>602</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="F113" s="4" t="s">
-        <v>100</v>
+        <v>605</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="B114" s="2" t="s">
-        <v>682</v>
+        <v>670</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>683</v>
+        <v>671</v>
       </c>
       <c r="F114" s="14" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>654</v>
+        <v>452</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>655</v>
+        <v>453</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>454</v>
       </c>
       <c r="F115" s="4" t="s">
         <v>100</v>
@@ -4948,41 +4972,41 @@
         <v>43</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>656</v>
+        <v>682</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+        <v>683</v>
+      </c>
+      <c r="F116" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>575</v>
+        <v>654</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>576</v>
+        <v>655</v>
       </c>
       <c r="F117" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="F118" s="3" t="s">
-        <v>99</v>
+        <v>657</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -4990,102 +5014,96 @@
         <v>43</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>599</v>
+        <v>575</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>576</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>742</v>
+        <v>652</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>744</v>
+        <v>653</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="F121" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="17" t="s">
+      <c r="F123" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B122" s="17" t="s">
+      <c r="B124" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="C122" s="17" t="s">
+      <c r="C124" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="D122" s="17" t="s">
+      <c r="D124" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="E122" s="17"/>
-      <c r="F122" s="21" t="s">
+      <c r="E124" s="17"/>
+      <c r="F124" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G122" s="17" t="s">
+      <c r="G124" s="17" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="F123" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="F124" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -5093,10 +5111,13 @@
         <v>275</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>710</v>
       </c>
       <c r="F125" s="4" t="s">
         <v>100</v>
@@ -5107,13 +5128,16 @@
         <v>275</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>418</v>
+        <v>273</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="F126" s="5" t="s">
-        <v>101</v>
+        <v>274</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="F126" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -5121,103 +5145,100 @@
         <v>275</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>183</v>
+        <v>271</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>182</v>
+        <v>272</v>
       </c>
       <c r="F127" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>184</v>
+        <v>418</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F128" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F129" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="B129" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C129" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="D129" s="17"/>
-      <c r="E129" s="17"/>
-      <c r="F129" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G129" s="17"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>55</v>
+        <v>275</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>471</v>
+        <v>184</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="B131" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C131" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G131" s="17"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>380</v>
+        <v>471</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>381</v>
+        <v>472</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>56</v>
+        <v>473</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>59</v>
+        <v>474</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>268</v>
+        <v>475</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>99</v>
@@ -5228,30 +5249,30 @@
         <v>55</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>313</v>
+        <v>380</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F134" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>526</v>
+        <v>56</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="F135" s="5" t="s">
-        <v>101</v>
+        <v>59</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -5259,13 +5280,13 @@
         <v>55</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>544</v>
+        <v>313</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="F136" s="3" t="s">
-        <v>99</v>
+        <v>314</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -5273,30 +5294,30 @@
         <v>55</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>610</v>
+        <v>526</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="F137" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>527</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>57</v>
+        <v>544</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F138" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>337</v>
+        <v>545</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -5304,13 +5325,13 @@
         <v>55</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>311</v>
+        <v>610</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F139" s="5" t="s">
-        <v>101</v>
+        <v>611</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5318,33 +5339,30 @@
         <v>55</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>390</v>
+        <v>57</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="F140" s="16" t="s">
-        <v>303</v>
+        <v>60</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>391</v>
+        <v>311</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="F141" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G141" s="2" t="s">
-        <v>397</v>
+        <v>312</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5352,142 +5370,148 @@
         <v>55</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F142" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>58</v>
+        <v>391</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F143" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+      <c r="F143" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>376</v>
+        <v>392</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F144" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+      <c r="F144" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>388</v>
+        <v>58</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>389</v>
+        <v>61</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="F145" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B146" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="F146" s="6" t="s">
+      <c r="F148" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G146" s="2" t="s">
+      <c r="G148" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="24" t="s">
+    <row r="149" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="B147" s="24" t="s">
+      <c r="B149" s="24" t="s">
         <v>406</v>
       </c>
-      <c r="C147" s="24" t="s">
+      <c r="C149" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="D147" s="24" t="s">
+      <c r="D149" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="E147" s="24"/>
-      <c r="F147" s="19" t="s">
+      <c r="E149" s="24"/>
+      <c r="F149" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G147" s="24"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A148" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="F148" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A149" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F149" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="G149" s="24"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F150" s="4" t="s">
-        <v>100</v>
+        <v>366</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -5495,13 +5519,10 @@
         <v>357</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F151" s="4" t="s">
         <v>100</v>
@@ -5512,10 +5533,10 @@
         <v>357</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>100</v>
@@ -5526,98 +5547,95 @@
         <v>357</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F153" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G153" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F153" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B154" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F154" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="F154" s="6" t="s">
+      <c r="F156" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G154" s="2" t="s">
+      <c r="G156" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="17" t="s">
+    <row r="157" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B155" s="17" t="s">
+      <c r="B157" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="C155" s="17" t="s">
+      <c r="C157" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="D155" s="17"/>
-      <c r="E155" s="17"/>
-      <c r="F155" s="20" t="s">
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G155" s="17"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A156" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F156" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A157" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="F157" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G157" s="17"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>667</v>
+        <v>206</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="F158" s="4" t="s">
-        <v>100</v>
+        <v>207</v>
+      </c>
+      <c r="F158" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5625,19 +5643,16 @@
         <v>63</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>197</v>
+        <v>519</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F159" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G159" s="2" t="s">
-        <v>339</v>
+        <v>520</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="F159" s="14" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5645,13 +5660,16 @@
         <v>63</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>326</v>
+        <v>667</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F160" s="5" t="s">
-        <v>101</v>
+        <v>668</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="F160" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5659,44 +5677,47 @@
         <v>63</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F161" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F161" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G161" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>497</v>
+        <v>326</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>498</v>
+        <v>327</v>
       </c>
       <c r="F162" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F163" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G163" s="2" t="s">
-        <v>345</v>
+        <v>67</v>
+      </c>
+      <c r="F163" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -5704,30 +5725,30 @@
         <v>63</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>564</v>
+        <v>498</v>
       </c>
       <c r="F164" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>516</v>
+        <v>65</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="F165" s="6" t="s">
-        <v>102</v>
+        <v>68</v>
+      </c>
+      <c r="F165" s="16" t="s">
+        <v>303</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>518</v>
+        <v>345</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5735,30 +5756,30 @@
         <v>63</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>199</v>
+        <v>563</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F166" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>564</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>66</v>
+        <v>516</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F167" s="14" t="s">
-        <v>400</v>
+        <v>517</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5766,10 +5787,10 @@
         <v>63</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="F168" s="4" t="s">
         <v>100</v>
@@ -5780,27 +5801,30 @@
         <v>63</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>277</v>
+        <v>66</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F169" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F169" s="14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>278</v>
+        <v>190</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F170" s="5" t="s">
-        <v>101</v>
+        <v>191</v>
+      </c>
+      <c r="F170" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5808,13 +5832,13 @@
         <v>63</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F171" s="4" t="s">
-        <v>100</v>
+        <v>280</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -5822,24 +5846,24 @@
         <v>63</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>568</v>
+        <v>278</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>569</v>
+        <v>281</v>
       </c>
       <c r="F172" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>477</v>
+        <v>279</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>476</v>
+        <v>282</v>
       </c>
       <c r="F173" s="4" t="s">
         <v>100</v>
@@ -5850,75 +5874,72 @@
         <v>63</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>493</v>
+        <v>568</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="F174" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="F174" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A175" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="F175" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B175" s="17" t="s">
-        <v>495</v>
-      </c>
-      <c r="C175" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="D175" s="17"/>
-      <c r="E175" s="17"/>
-      <c r="F175" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G175" s="17"/>
     </row>
     <row r="176" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>420</v>
+        <v>63</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>560</v>
+        <v>493</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="F176" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A177" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>715</v>
-      </c>
-      <c r="F177" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+        <v>494</v>
+      </c>
+      <c r="F176" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A177" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B177" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="C177" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G177" s="17"/>
+    </row>
+    <row r="178" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>428</v>
+        <v>560</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>429</v>
+        <v>561</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>562</v>
       </c>
       <c r="F178" s="3" t="s">
         <v>99</v>
@@ -5929,10 +5950,13 @@
         <v>420</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>430</v>
+        <v>716</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>431</v>
+        <v>717</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>715</v>
       </c>
       <c r="F179" s="3" t="s">
         <v>99</v>
@@ -5943,10 +5967,10 @@
         <v>420</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>401</v>
+        <v>428</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>402</v>
+        <v>429</v>
       </c>
       <c r="F180" s="3" t="s">
         <v>99</v>
@@ -5957,30 +5981,24 @@
         <v>420</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F181" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>616</v>
+        <v>401</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="D182" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="E182" s="2" t="s">
-        <v>434</v>
+        <v>402</v>
       </c>
       <c r="F182" s="3" t="s">
         <v>99</v>
@@ -5991,107 +6009,110 @@
         <v>420</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>422</v>
+        <v>616</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>424</v>
+        <v>618</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>531</v>
+        <v>434</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="F185" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G185" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>480</v>
+        <v>422</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="F186" s="3"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+        <v>424</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="F187" s="6" t="s">
-        <v>142</v>
+        <v>532</v>
+      </c>
+      <c r="F187" s="16" t="s">
+        <v>303</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="E188" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="F188" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>481</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F188" s="3"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>501</v>
+        <v>529</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="F189" s="5" t="s">
-        <v>101</v>
+        <v>530</v>
+      </c>
+      <c r="F189" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -6099,13 +6120,16 @@
         <v>420</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>467</v>
+        <v>503</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="F190" s="5" t="s">
-        <v>101</v>
+        <v>504</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -6113,10 +6137,10 @@
         <v>420</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>423</v>
+        <v>501</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>425</v>
+        <v>502</v>
       </c>
       <c r="F191" s="5" t="s">
         <v>101</v>
@@ -6127,10 +6151,10 @@
         <v>420</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F192" s="5" t="s">
         <v>101</v>
@@ -6141,151 +6165,151 @@
         <v>420</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>542</v>
+        <v>423</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="F193" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>426</v>
+        <v>469</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="F194" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G194" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>470</v>
+      </c>
+      <c r="F194" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B195" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F196" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G196" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A197" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C197" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="F195" s="19" t="s">
+      <c r="F197" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="17" t="s">
+    <row r="198" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="B196" s="17" t="s">
+      <c r="B198" s="17" t="s">
         <v>491</v>
       </c>
-      <c r="C196" s="17" t="s">
+      <c r="C198" s="17" t="s">
         <v>492</v>
       </c>
-      <c r="D196" s="17"/>
-      <c r="E196" s="17"/>
-      <c r="F196" s="19" t="s">
+      <c r="D198" s="17"/>
+      <c r="E198" s="17"/>
+      <c r="F198" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G196" s="17"/>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A197" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F197" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A198" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F198" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G198" s="17"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F199" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>213</v>
+        <v>304</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F200" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G200" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F200" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F201" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>94</v>
+        <v>213</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F202" s="5" t="s">
-        <v>101</v>
+        <v>214</v>
+      </c>
+      <c r="F202" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -6293,142 +6317,142 @@
         <v>93</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F203" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+      <c r="F203" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>218</v>
+        <v>94</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F204" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A205" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B205" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C205" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D205" s="17"/>
-      <c r="E205" s="17"/>
-      <c r="F205" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G205" s="17"/>
+      <c r="B205" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="206" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>71</v>
+        <v>218</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F206" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G206" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A207" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F207" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G207" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+      <c r="F206" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A207" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B207" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C207" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D207" s="17"/>
+      <c r="E207" s="17"/>
+      <c r="F207" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G207" s="17"/>
+    </row>
+    <row r="208" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>751</v>
+        <v>71</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>752</v>
+        <v>72</v>
       </c>
       <c r="F208" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A209" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F209" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G208" s="2" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A209" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B209" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C209" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D209" s="17"/>
-      <c r="E209" s="17"/>
-      <c r="F209" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="G209" s="17" t="s">
-        <v>336</v>
+      <c r="G209" s="2" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>635</v>
+        <v>751</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="F210" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A211" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>101</v>
+        <v>752</v>
+      </c>
+      <c r="F210" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G210" s="2" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A211" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B211" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C211" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D211" s="17"/>
+      <c r="E211" s="17"/>
+      <c r="F211" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G211" s="17" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -6436,10 +6460,10 @@
         <v>73</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>74</v>
+        <v>635</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>82</v>
+        <v>636</v>
       </c>
       <c r="F212" s="4" t="s">
         <v>100</v>
@@ -6450,27 +6474,27 @@
         <v>73</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>75</v>
+        <v>551</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>83</v>
+        <v>552</v>
       </c>
       <c r="F213" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>555</v>
+        <v>74</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="F214" s="5" t="s">
-        <v>101</v>
+        <v>82</v>
+      </c>
+      <c r="F214" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -6478,27 +6502,27 @@
         <v>73</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>411</v>
+        <v>75</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="F215" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="F215" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>680</v>
+        <v>555</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="F216" s="4" t="s">
-        <v>100</v>
+        <v>556</v>
+      </c>
+      <c r="F216" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -6506,13 +6530,13 @@
         <v>73</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>553</v>
+        <v>411</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="F217" s="5" t="s">
-        <v>101</v>
+        <v>412</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -6520,13 +6544,13 @@
         <v>73</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>283</v>
+        <v>680</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F218" s="3" t="s">
-        <v>99</v>
+        <v>681</v>
+      </c>
+      <c r="F218" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -6534,30 +6558,27 @@
         <v>73</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>256</v>
+        <v>553</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F219" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="220" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>554</v>
+      </c>
+      <c r="F219" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>236</v>
+        <v>283</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E220" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F220" s="5" t="s">
-        <v>101</v>
+        <v>284</v>
+      </c>
+      <c r="F220" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -6565,24 +6586,27 @@
         <v>73</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>621</v>
+        <v>256</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="F221" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="F221" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>623</v>
+        <v>236</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>624</v>
+        <v>237</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="F222" s="5" t="s">
         <v>101</v>
@@ -6593,10 +6617,10 @@
         <v>73</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>232</v>
+        <v>621</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>233</v>
+        <v>622</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>101</v>
@@ -6607,10 +6631,10 @@
         <v>73</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>228</v>
+        <v>623</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>229</v>
+        <v>624</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>101</v>
@@ -6621,13 +6645,10 @@
         <v>73</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>637</v>
+        <v>232</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="D225" s="2" t="s">
-        <v>639</v>
+        <v>233</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>101</v>
@@ -6638,10 +6659,10 @@
         <v>73</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>625</v>
+        <v>228</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>626</v>
+        <v>229</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>101</v>
@@ -6652,13 +6673,16 @@
         <v>73</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>713</v>
+        <v>637</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="F227" s="3" t="s">
-        <v>99</v>
+        <v>638</v>
+      </c>
+      <c r="D227" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="F227" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -6666,13 +6690,13 @@
         <v>73</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="F228" s="3" t="s">
-        <v>99</v>
+        <v>626</v>
+      </c>
+      <c r="F228" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -6680,10 +6704,10 @@
         <v>73</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>612</v>
+        <v>713</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>613</v>
+        <v>714</v>
       </c>
       <c r="F229" s="3" t="s">
         <v>99</v>
@@ -6694,13 +6718,13 @@
         <v>73</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>590</v>
+        <v>640</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="F230" s="4" t="s">
-        <v>100</v>
+        <v>641</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -6708,30 +6732,27 @@
         <v>73</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>241</v>
+        <v>612</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F231" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>613</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>285</v>
+        <v>590</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F232" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G232" s="2" t="s">
-        <v>334</v>
+        <v>591</v>
+      </c>
+      <c r="F232" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -6739,27 +6760,30 @@
         <v>73</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>76</v>
+        <v>241</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F233" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="F233" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>77</v>
+        <v>285</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F234" s="5" t="s">
-        <v>101</v>
+        <v>286</v>
+      </c>
+      <c r="F234" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G234" s="2" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -6767,10 +6791,10 @@
         <v>73</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F235" s="5" t="s">
         <v>101</v>
@@ -6781,13 +6805,13 @@
         <v>73</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F236" s="4" t="s">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="F236" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -6795,13 +6819,10 @@
         <v>73</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>627</v>
+        <v>78</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>629</v>
+        <v>86</v>
       </c>
       <c r="F237" s="5" t="s">
         <v>101</v>
@@ -6812,10 +6833,10 @@
         <v>73</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>448</v>
+        <v>79</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>449</v>
+        <v>87</v>
       </c>
       <c r="F238" s="4" t="s">
         <v>100</v>
@@ -6826,27 +6847,30 @@
         <v>73</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>478</v>
+        <v>627</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F239" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="240" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>628</v>
+      </c>
+      <c r="D239" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="F239" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>642</v>
+        <v>448</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="F240" s="5" t="s">
-        <v>101</v>
+        <v>449</v>
+      </c>
+      <c r="F240" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -6854,27 +6878,27 @@
         <v>73</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>745</v>
+        <v>478</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="F241" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+        <v>479</v>
+      </c>
+      <c r="F241" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>80</v>
+        <v>642</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F242" s="3" t="s">
-        <v>99</v>
+        <v>643</v>
+      </c>
+      <c r="F242" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -6882,47 +6906,41 @@
         <v>73</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>549</v>
+        <v>745</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="F243" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>746</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F244" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G244" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>295</v>
+        <v>549</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F245" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G245" s="2" t="s">
-        <v>335</v>
+        <v>550</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -6930,10 +6948,10 @@
         <v>73</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>240</v>
+        <v>294</v>
       </c>
       <c r="F246" s="16" t="s">
         <v>303</v>
@@ -6942,80 +6960,83 @@
         <v>335</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>230</v>
+        <v>295</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E247" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F247" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+      <c r="F247" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G247" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>696</v>
+        <v>239</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="F248" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+      <c r="F248" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G248" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>81</v>
+        <v>230</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>89</v>
+        <v>231</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F249" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>749</v>
+        <v>696</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>750</v>
-      </c>
-      <c r="F250" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>697</v>
+      </c>
+      <c r="F250" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>443</v>
+        <v>81</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F251" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G251" s="2" t="s">
-        <v>377</v>
+        <v>89</v>
+      </c>
+      <c r="F251" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -7023,27 +7044,30 @@
         <v>73</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>644</v>
+        <v>749</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="F252" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+        <v>750</v>
+      </c>
+      <c r="F252" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>507</v>
+        <v>443</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="F253" s="5" t="s">
-        <v>101</v>
+        <v>444</v>
+      </c>
+      <c r="F253" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G253" s="2" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -7051,13 +7075,13 @@
         <v>73</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>245</v>
+        <v>644</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F254" s="14" t="s">
-        <v>258</v>
+        <v>645</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -7065,10 +7089,10 @@
         <v>73</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>298</v>
+        <v>507</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>297</v>
+        <v>508</v>
       </c>
       <c r="F255" s="5" t="s">
         <v>101</v>
@@ -7079,13 +7103,13 @@
         <v>73</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>646</v>
+        <v>245</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="F256" s="4" t="s">
-        <v>100</v>
+        <v>246</v>
+      </c>
+      <c r="F256" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -7093,10 +7117,10 @@
         <v>73</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>234</v>
+        <v>298</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>235</v>
+        <v>297</v>
       </c>
       <c r="F257" s="5" t="s">
         <v>101</v>
@@ -7107,13 +7131,13 @@
         <v>73</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>630</v>
+        <v>646</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="F258" s="5" t="s">
-        <v>101</v>
+        <v>647</v>
+      </c>
+      <c r="F258" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -7121,13 +7145,13 @@
         <v>73</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F259" s="12" t="s">
-        <v>250</v>
+        <v>235</v>
+      </c>
+      <c r="F259" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -7135,13 +7159,13 @@
         <v>73</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>524</v>
+        <v>630</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F260" s="14" t="s">
-        <v>258</v>
+        <v>631</v>
+      </c>
+      <c r="F260" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -7149,16 +7173,13 @@
         <v>73</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>522</v>
+        <v>226</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E261" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F261" s="5" t="s">
-        <v>101</v>
+        <v>227</v>
+      </c>
+      <c r="F261" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -7166,126 +7187,123 @@
         <v>73</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>224</v>
+        <v>524</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F262" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="263" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>525</v>
+      </c>
+      <c r="F262" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>648</v>
+        <v>522</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="F263" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="264" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>523</v>
+      </c>
+      <c r="E263" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F263" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>585</v>
+        <v>224</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="F264" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G264" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="265" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+      <c r="F264" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A265" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B265" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="F265" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A266" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F266" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G266" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A267" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B267" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="C267" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F265" s="16" t="s">
+      <c r="F267" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G265" s="2" t="s">
+      <c r="G267" s="2" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A266" s="17" t="s">
+    <row r="268" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A268" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B266" s="17" t="s">
+      <c r="B268" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="C266" s="17" t="s">
+      <c r="C268" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="D266" s="17"/>
-      <c r="E266" s="17"/>
-      <c r="F266" s="20" t="s">
+      <c r="D268" s="17"/>
+      <c r="E268" s="17"/>
+      <c r="F268" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G266" s="17"/>
-    </row>
-    <row r="267" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A267" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B267" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D267" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F267" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B268" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D268" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="F268" s="5" t="s">
-        <v>101</v>
-      </c>
+      <c r="G268" s="17"/>
     </row>
     <row r="269" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>247</v>
+        <v>91</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>248</v>
+        <v>92</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>249</v>
+        <v>315</v>
       </c>
       <c r="F269" s="5" t="s">
         <v>101</v>
@@ -7296,50 +7314,84 @@
         <v>90</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>351</v>
+        <v>222</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F270" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+      <c r="D270" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="F270" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B271" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F271" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A272" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F272" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A273" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B273" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="C273" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="D271" s="2" t="s">
+      <c r="D273" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="F271" s="4" t="s">
+      <c r="F273" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A272" s="17" t="s">
+    <row r="274" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A274" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B272" s="17" t="s">
+      <c r="B274" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="C272" s="17" t="s">
+      <c r="C274" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D272" s="17" t="s">
+      <c r="D274" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="E272" s="17"/>
-      <c r="F272" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G272" s="17"/>
+      <c r="E274" s="17"/>
+      <c r="F274" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G274" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to U.S. develop commit #d300b00a
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AD8C04-7187-4F7D-AEBA-76C1921E8978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE41482-7AAD-4FF8-8F3A-C46659165C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="769">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2336,6 +2336,9 @@
   </si>
   <si>
     <t>Capacity Supply Curve Capacity Cost Multiplier vs Share of Exisiting Capacity Built This Year, Capacity Supply Curve Minimum Buildable Capacity for Plant Types with No Exisiting Capacity, Capacity Supply Curve Share of Cost Effective Capacity Built in a Single Year, Capacity Supply Curve Share of Cost Effective Hybrid Capacity Built in a Single Year</t>
+  </si>
+  <si>
+    <t>BAU RPS Alternative Compliance Payment, RPS Alternative Compliance Payment</t>
   </si>
 </sst>
 </file>
@@ -2438,7 +2441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2496,12 +2499,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2815,7 +2812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -3151,9 +3148,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G275"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4084,52 +4081,50 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="17" t="s">
         <v>464</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="17" t="s">
         <v>465</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="17" t="s">
         <v>726</v>
       </c>
-      <c r="F59" s="6" t="s">
+      <c r="E59" s="17"/>
+      <c r="F59" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="17" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
-        <v>413</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>753</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>754</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G60" s="17"/>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>99</v>
@@ -4140,13 +4135,13 @@
         <v>38</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>201</v>
+        <v>40</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>99</v>
+        <v>42</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -4154,46 +4149,49 @@
         <v>38</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>40</v>
+        <v>546</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>42</v>
+        <v>547</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B65" s="17" t="s">
+      <c r="B64" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C64" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="21" t="s">
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4201,61 +4199,61 @@
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>658</v>
+        <v>181</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>659</v>
+        <v>727</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>728</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>181</v>
+        <v>328</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>728</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>328</v>
+        <v>604</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>604</v>
+        <v>687</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>101</v>
+        <v>688</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4263,33 +4261,33 @@
         <v>43</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>687</v>
+        <v>175</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>689</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>175</v>
+        <v>595</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>320</v>
+        <v>596</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4297,30 +4295,30 @@
         <v>43</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>595</v>
+        <v>44</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>99</v>
+        <v>51</v>
+      </c>
+      <c r="F73" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -4328,78 +4326,75 @@
         <v>43</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>45</v>
+        <v>757</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>758</v>
       </c>
       <c r="F74" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>757</v>
+        <v>694</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>758</v>
-      </c>
-      <c r="F75" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>695</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>694</v>
+        <v>677</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>695</v>
+        <v>678</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>677</v>
+        <v>692</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>203</v>
+        <v>693</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>692</v>
+        <v>160</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>693</v>
+        <v>161</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>99</v>
@@ -4410,106 +4405,106 @@
         <v>43</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>160</v>
+        <v>661</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>662</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>661</v>
+        <v>46</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>662</v>
+        <v>52</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>730</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>46</v>
+        <v>731</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>731</v>
+        <v>513</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>732</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>513</v>
+        <v>733</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>734</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>733</v>
+        <v>650</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>767</v>
+        <v>651</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>650</v>
+        <v>309</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>101</v>
+        <v>310</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4517,27 +4512,30 @@
         <v>43</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>309</v>
+        <v>746</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>310</v>
+        <v>747</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>746</v>
+        <v>47</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>100</v>
+        <v>171</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4545,16 +4543,16 @@
         <v>43</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>47</v>
+        <v>288</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>99</v>
+        <v>290</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4562,16 +4560,16 @@
         <v>43</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>288</v>
+        <v>663</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>289</v>
+        <v>664</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>100</v>
+        <v>735</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4579,154 +4577,151 @@
         <v>43</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>663</v>
+        <v>169</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>664</v>
+        <v>170</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>169</v>
+        <v>674</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>170</v>
+        <v>675</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>674</v>
+        <v>608</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>608</v>
+        <v>736</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>609</v>
+        <v>737</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>736</v>
+        <v>489</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>737</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>489</v>
+        <v>177</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>177</v>
+        <v>718</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>718</v>
+        <v>738</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>719</v>
+        <v>739</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>738</v>
+        <v>593</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>739</v>
+        <v>594</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>593</v>
+        <v>606</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>100</v>
+        <v>607</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4734,10 +4729,10 @@
         <v>43</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>606</v>
+        <v>755</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>607</v>
+        <v>756</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>99</v>
@@ -4748,13 +4743,13 @@
         <v>43</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>755</v>
+        <v>597</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>99</v>
+        <v>598</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4762,10 +4757,10 @@
         <v>43</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>597</v>
+        <v>665</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>598</v>
+        <v>666</v>
       </c>
       <c r="F102" s="4" t="s">
         <v>100</v>
@@ -4776,13 +4771,13 @@
         <v>43</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>665</v>
+        <v>48</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="F103" s="4" t="s">
-        <v>100</v>
+        <v>53</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4790,27 +4785,30 @@
         <v>43</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>196</v>
+        <v>49</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F105" s="4" t="s">
-        <v>100</v>
+        <v>54</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4818,33 +4816,33 @@
         <v>43</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>49</v>
+        <v>760</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>54</v>
+        <v>761</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>102</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="F107" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>762</v>
+        <v>754</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5485,20 +5483,20 @@
         <v>353</v>
       </c>
     </row>
-    <row r="149" spans="1:7" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="25" t="s">
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B149" s="25" t="s">
+      <c r="B149" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C149" s="25" t="s">
+      <c r="C149" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="D149" s="25" t="s">
+      <c r="D149" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="F149" s="26" t="s">
+      <c r="F149" s="3" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Copy in EU-2024-develop branch
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8129B8F3-CD5F-469F-8564-550C965CF605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE41482-7AAD-4FF8-8F3A-C46659165C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1322" uniqueCount="769">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -2104,12 +2104,6 @@
     <t>Fraction of EVs Used for Grid Balancing on Average Day, Fraction of EV Battery Capacity Used for Grid Balancing when EV is Used for Grid Balancing</t>
   </si>
   <si>
-    <t>DATAiRC</t>
-  </si>
-  <si>
-    <t>Demand-Altering Technology Assistance in RPS Compliance</t>
-  </si>
-  <si>
     <t>CCSTaSC</t>
   </si>
   <si>
@@ -2134,15 +2128,6 @@
     <t>Non-Battery Portion of New Vehicle Prices</t>
   </si>
   <si>
-    <t>SoEIaEbH</t>
-  </si>
-  <si>
-    <t>Share of Electricity Imports and Exports by Hour</t>
-  </si>
-  <si>
-    <t>Share of Electricity Imports by Hour, Share of Electricity Exports by Hour</t>
-  </si>
-  <si>
     <t>CO2 Capture Potential by Electricity Source, CO2 Capture Potential by Industry,CO2 Capture Potential by Hydrogen Sector</t>
   </si>
   <si>
@@ -2254,9 +2239,6 @@
     <t>Capacity Supply Curve</t>
   </si>
   <si>
-    <t>Capacity Supply Curve Capacity Cost Multiplier vs Share of Exisiting Capacity Built This Year, Capacity Supply Curve Minimum Buildable Capacity for Plant Types with No Exisiting Capacity, Capacity Supply Curve Share of Cost Effective Capacity Built in a Single Year</t>
-  </si>
-  <si>
     <t>Electricity Dispatch Weibull Parameter A, Electricity Dispatch Weibull Parameter B</t>
   </si>
   <si>
@@ -2315,6 +2297,48 @@
   </si>
   <si>
     <t>RPS Alternative Compliance Payment</t>
+  </si>
+  <si>
+    <t>MaMHEIaE</t>
+  </si>
+  <si>
+    <t>Max and Min Hourly Electriicty Imports and Exports</t>
+  </si>
+  <si>
+    <t>BPMCRS</t>
+  </si>
+  <si>
+    <t>BAU Policy Mandated Capacity Retrofit Schedule</t>
+  </si>
+  <si>
+    <t>You know particular capacities of particular types of plants will be retrofit with CCUS in particular years (for example, they are already under construction), or you are modeling a region where power plant retrofit decisions are based on government mandates rather than being market-driven</t>
+  </si>
+  <si>
+    <t>PMCRS</t>
+  </si>
+  <si>
+    <t>Policy Mandated Capacity Retrofit Schedule</t>
+  </si>
+  <si>
+    <t>You are modeling a region where power plant CCUS retrofit decisions are based on government mandates rather than being market-driven, and you are setting this policy lever to alter the BAU mandates</t>
+  </si>
+  <si>
+    <t>goeeng</t>
+  </si>
+  <si>
+    <t>ERWD</t>
+  </si>
+  <si>
+    <t>Enhanced Rock Weathering Data</t>
+  </si>
+  <si>
+    <t>Enhanced Rock Weathering Potential, Enhanced Rock Weathering Energy Intensity, Enhanced Rock Weathering Amortized CapEx and OM</t>
+  </si>
+  <si>
+    <t>Capacity Supply Curve Capacity Cost Multiplier vs Share of Exisiting Capacity Built This Year, Capacity Supply Curve Minimum Buildable Capacity for Plant Types with No Exisiting Capacity, Capacity Supply Curve Share of Cost Effective Capacity Built in a Single Year, Capacity Supply Curve Share of Cost Effective Hybrid Capacity Built in a Single Year</t>
+  </si>
+  <si>
+    <t>BAU RPS Alternative Compliance Payment, RPS Alternative Compliance Payment</t>
   </si>
 </sst>
 </file>
@@ -2396,7 +2420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2413,22 +2437,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2483,9 +2496,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2802,7 +2812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -3136,11 +3146,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G273"/>
+  <dimension ref="A1:G275"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3193,7 +3203,7 @@
       <c r="F2" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>541</v>
       </c>
     </row>
@@ -3309,10 +3319,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>99</v>
@@ -3702,13 +3712,13 @@
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>101</v>
@@ -3719,10 +3729,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>100</v>
@@ -3739,7 +3749,7 @@
         <v>417</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>101</v>
@@ -3756,7 +3766,7 @@
         <v>410</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>101</v>
@@ -3767,10 +3777,10 @@
         <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>101</v>
@@ -3781,10 +3791,10 @@
         <v>36</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>100</v>
@@ -3798,7 +3808,7 @@
         <v>575</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="F42" s="20" t="s">
         <v>100</v>
@@ -3853,7 +3863,7 @@
         <v>142</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3946,16 +3956,16 @@
         <v>413</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>180</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4071,52 +4081,50 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="17" t="s">
         <v>464</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="17" t="s">
         <v>465</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>731</v>
-      </c>
-      <c r="F59" s="6" t="s">
+      <c r="D59" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="17" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
-        <v>413</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>759</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>760</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G60" s="17"/>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>99</v>
@@ -4127,13 +4135,13 @@
         <v>38</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>201</v>
+        <v>40</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>99</v>
+        <v>42</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -4141,46 +4149,49 @@
         <v>38</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>40</v>
+        <v>546</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>42</v>
+        <v>547</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B65" s="17" t="s">
+      <c r="B64" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C64" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="21" t="s">
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4188,61 +4199,61 @@
         <v>43</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>658</v>
+        <v>181</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>659</v>
+        <v>727</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>728</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>181</v>
+        <v>328</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>732</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>733</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>328</v>
+        <v>604</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>604</v>
+        <v>687</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>101</v>
+        <v>688</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4250,33 +4261,33 @@
         <v>43</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>687</v>
+        <v>175</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>688</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>689</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>175</v>
+        <v>595</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>320</v>
+        <v>596</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4284,30 +4295,30 @@
         <v>43</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>595</v>
+        <v>44</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="F72" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>99</v>
+        <v>51</v>
+      </c>
+      <c r="F73" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -4315,16 +4326,16 @@
         <v>43</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>45</v>
+        <v>757</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>51</v>
+        <v>758</v>
       </c>
       <c r="F74" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>322</v>
+        <v>759</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4332,10 +4343,10 @@
         <v>43</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>99</v>
@@ -4366,10 +4377,10 @@
         <v>43</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>99</v>
@@ -4414,7 +4425,7 @@
         <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>101</v>
@@ -4425,10 +4436,10 @@
         <v>43</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>101</v>
@@ -4451,18 +4462,18 @@
         <v>515</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>740</v>
+        <v>767</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>101</v>
@@ -4473,27 +4484,27 @@
         <v>43</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>690</v>
+        <v>650</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F84" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>650</v>
+        <v>309</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>101</v>
+        <v>310</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4501,27 +4512,30 @@
         <v>43</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>309</v>
+        <v>746</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>310</v>
+        <v>747</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>752</v>
+        <v>47</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>100</v>
+        <v>171</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4529,16 +4543,16 @@
         <v>43</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>47</v>
+        <v>288</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>713</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>99</v>
+        <v>290</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4546,16 +4560,16 @@
         <v>43</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>288</v>
+        <v>663</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>289</v>
+        <v>664</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>100</v>
+        <v>735</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4563,154 +4577,151 @@
         <v>43</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>663</v>
+        <v>169</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>664</v>
+        <v>170</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>169</v>
+        <v>674</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>170</v>
+        <v>675</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>674</v>
+        <v>608</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>608</v>
+        <v>736</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>609</v>
+        <v>737</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>742</v>
+        <v>489</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>743</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>489</v>
+        <v>177</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>177</v>
+        <v>718</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="F96" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>719</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>723</v>
+        <v>738</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>744</v>
+        <v>593</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>745</v>
+        <v>594</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>593</v>
+        <v>606</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>100</v>
+        <v>607</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4718,10 +4729,10 @@
         <v>43</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>606</v>
+        <v>755</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>607</v>
+        <v>756</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>99</v>
@@ -4800,111 +4811,117 @@
         <v>323</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>672</v>
+        <v>760</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>746</v>
-      </c>
-      <c r="F106" s="14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+        <v>761</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>186</v>
+        <v>753</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>754</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>580</v>
+        <v>672</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="F108" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>684</v>
+        <v>580</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>601</v>
+        <v>203</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>602</v>
+        <v>204</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B112" s="2" t="s">
-        <v>670</v>
+        <v>684</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="F112" s="14" t="s">
-        <v>258</v>
+        <v>685</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4912,47 +4929,44 @@
         <v>43</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>700</v>
+        <v>601</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>701</v>
+        <v>602</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>702</v>
+        <v>605</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>452</v>
+        <v>670</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>671</v>
+      </c>
+      <c r="F114" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>682</v>
+        <v>452</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="F115" s="14" t="s">
-        <v>258</v>
+        <v>453</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4960,13 +4974,13 @@
         <v>43</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>654</v>
+        <v>682</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>100</v>
+        <v>683</v>
+      </c>
+      <c r="F116" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4974,10 +4988,10 @@
         <v>43</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F117" s="4" t="s">
         <v>100</v>
@@ -4988,27 +5002,27 @@
         <v>43</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>575</v>
+        <v>656</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>576</v>
+        <v>657</v>
       </c>
       <c r="F118" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>652</v>
+        <v>575</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>99</v>
+        <v>576</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -5016,30 +5030,27 @@
         <v>43</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>599</v>
+        <v>652</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>597</v>
+        <v>653</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>747</v>
+        <v>599</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>749</v>
+        <v>600</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>597</v>
       </c>
       <c r="F121" s="3" t="s">
         <v>99</v>
@@ -5050,51 +5061,51 @@
         <v>43</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>716</v>
+        <v>741</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="F122" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="17" t="s">
+        <v>742</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B123" s="17" t="s">
+      <c r="B123" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B124" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="C123" s="17" t="s">
+      <c r="C124" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="D123" s="17" t="s">
+      <c r="D124" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="E123" s="17"/>
-      <c r="F123" s="21" t="s">
+      <c r="E124" s="17"/>
+      <c r="F124" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="G123" s="17" t="s">
+      <c r="G124" s="17" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>715</v>
-      </c>
-      <c r="F124" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5102,117 +5113,117 @@
         <v>275</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>634</v>
+        <v>710</v>
       </c>
       <c r="F125" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>634</v>
       </c>
       <c r="F126" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>418</v>
+        <v>271</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>183</v>
+        <v>418</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F128" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F129" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="17" t="s">
+    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B130" s="17" t="s">
+      <c r="B130" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="B131" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="C130" s="17" t="s">
+      <c r="C131" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="D130" s="17"/>
-      <c r="E130" s="17"/>
-      <c r="F130" s="20" t="s">
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G130" s="17"/>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="G131" s="17"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>99</v>
@@ -5223,44 +5234,47 @@
         <v>55</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>380</v>
+        <v>473</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>381</v>
+        <v>474</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="F133" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>56</v>
+        <v>380</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>268</v>
+        <v>381</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>313</v>
+        <v>56</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F135" s="5" t="s">
-        <v>101</v>
+        <v>59</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -5268,13 +5282,10 @@
         <v>55</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>526</v>
+        <v>313</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>528</v>
+        <v>314</v>
       </c>
       <c r="F136" s="5" t="s">
         <v>101</v>
@@ -5285,13 +5296,16 @@
         <v>55</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>99</v>
+        <v>527</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -5299,61 +5313,58 @@
         <v>55</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>610</v>
+        <v>544</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="F138" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>57</v>
+        <v>610</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F139" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+        <v>611</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>311</v>
+        <v>57</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F140" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>390</v>
+        <v>311</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="F141" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G141" s="2" t="s">
-        <v>396</v>
+        <v>312</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5361,16 +5372,16 @@
         <v>55</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F142" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5378,128 +5389,132 @@
         <v>55</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F143" s="16" t="s">
         <v>303</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>58</v>
+        <v>392</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F144" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+      <c r="F144" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>376</v>
+        <v>58</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>340</v>
+        <v>61</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F145" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="F146" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B147" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" s="17" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B148" s="17" t="s">
         <v>441</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C148" s="17" t="s">
         <v>442</v>
       </c>
-      <c r="F147" s="6" t="s">
+      <c r="F148" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="G147" s="2" t="s">
+      <c r="G148" s="17" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="24" t="s">
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B148" s="24" t="s">
+      <c r="B149" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C148" s="24" t="s">
+      <c r="C149" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="D148" s="24" t="s">
+      <c r="D149" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="E148" s="24"/>
-      <c r="F148" s="19" t="s">
+      <c r="F149" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G148" s="24"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="F149" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="F150" s="4" t="s">
-        <v>100</v>
+    </row>
+    <row r="150" spans="1:7" s="17" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="17" t="s">
+        <v>763</v>
+      </c>
+      <c r="B150" s="17" t="s">
+        <v>764</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>765</v>
+      </c>
+      <c r="D150" s="17" t="s">
+        <v>766</v>
+      </c>
+      <c r="F150" s="19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -5507,61 +5522,58 @@
         <v>357</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F151" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+      <c r="F151" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F153" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>357</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F154" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G154" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F154" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5569,81 +5581,78 @@
         <v>357</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F155" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F156" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G156" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="F155" s="6" t="s">
+      <c r="F157" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G155" s="2" t="s">
+      <c r="G157" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="17" t="s">
+    <row r="158" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B156" s="17" t="s">
+      <c r="B158" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="C156" s="17" t="s">
+      <c r="C158" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="D156" s="17"/>
-      <c r="E156" s="17"/>
-      <c r="F156" s="20" t="s">
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G156" s="17"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F157" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="F158" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G158" s="17"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>667</v>
+        <v>206</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="F159" s="4" t="s">
-        <v>100</v>
+        <v>207</v>
+      </c>
+      <c r="F159" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5651,19 +5660,16 @@
         <v>63</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>197</v>
+        <v>519</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F160" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G160" s="2" t="s">
-        <v>339</v>
+        <v>520</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="F160" s="14" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5671,13 +5677,16 @@
         <v>63</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>326</v>
+        <v>667</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="F161" s="5" t="s">
-        <v>101</v>
+        <v>668</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5685,44 +5694,47 @@
         <v>63</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F162" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G162" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>497</v>
+        <v>326</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>498</v>
+        <v>327</v>
       </c>
       <c r="F163" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F164" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G164" s="2" t="s">
-        <v>345</v>
+        <v>67</v>
+      </c>
+      <c r="F164" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -5730,30 +5742,30 @@
         <v>63</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>564</v>
+        <v>498</v>
       </c>
       <c r="F165" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>516</v>
+        <v>65</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="F166" s="6" t="s">
-        <v>102</v>
+        <v>68</v>
+      </c>
+      <c r="F166" s="16" t="s">
+        <v>303</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>518</v>
+        <v>345</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -5761,41 +5773,41 @@
         <v>63</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>199</v>
+        <v>563</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F167" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+      <c r="F167" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>66</v>
+        <v>516</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F168" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G168" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="F169" s="4" t="s">
         <v>100</v>
@@ -5806,13 +5818,16 @@
         <v>63</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>277</v>
+        <v>66</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F170" s="5" t="s">
-        <v>101</v>
+        <v>69</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F170" s="14" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5820,13 +5835,13 @@
         <v>63</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>278</v>
+        <v>190</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F171" s="5" t="s">
-        <v>101</v>
+        <v>191</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5834,13 +5849,13 @@
         <v>63</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F172" s="4" t="s">
-        <v>100</v>
+        <v>280</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5848,10 +5863,10 @@
         <v>63</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>568</v>
+        <v>278</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>569</v>
+        <v>281</v>
       </c>
       <c r="F173" s="5" t="s">
         <v>101</v>
@@ -5862,10 +5877,10 @@
         <v>63</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>477</v>
+        <v>279</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>476</v>
+        <v>282</v>
       </c>
       <c r="F174" s="4" t="s">
         <v>100</v>
@@ -5876,75 +5891,72 @@
         <v>63</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>493</v>
+        <v>568</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="F175" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="F176" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B176" s="17" t="s">
-        <v>495</v>
-      </c>
-      <c r="C176" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="D176" s="17"/>
-      <c r="E176" s="17"/>
-      <c r="F176" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G176" s="17"/>
     </row>
     <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>420</v>
+        <v>63</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>560</v>
+        <v>493</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="F177" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>721</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>722</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="F178" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+      <c r="F177" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B178" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="C178" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G178" s="17"/>
+    </row>
+    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>428</v>
+        <v>560</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>429</v>
+        <v>561</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>562</v>
       </c>
       <c r="F179" s="3" t="s">
         <v>99</v>
@@ -5955,10 +5967,13 @@
         <v>420</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>430</v>
+        <v>716</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>431</v>
+        <v>717</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>715</v>
       </c>
       <c r="F180" s="3" t="s">
         <v>99</v>
@@ -5969,10 +5984,10 @@
         <v>420</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>401</v>
+        <v>428</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>402</v>
+        <v>429</v>
       </c>
       <c r="F181" s="3" t="s">
         <v>99</v>
@@ -5983,30 +5998,24 @@
         <v>420</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F182" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>616</v>
+        <v>401</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="D183" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>434</v>
+        <v>402</v>
       </c>
       <c r="F183" s="3" t="s">
         <v>99</v>
@@ -6017,76 +6026,78 @@
         <v>420</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F184" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>422</v>
+        <v>616</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>424</v>
+        <v>618</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="F185" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>531</v>
+        <v>434</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="F186" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G186" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>480</v>
+        <v>422</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="D187" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="F187" s="3"/>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="F188" s="6" t="s">
-        <v>142</v>
+        <v>532</v>
+      </c>
+      <c r="F188" s="16" t="s">
+        <v>303</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6094,44 +6105,48 @@
         <v>420</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="E189" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="F189" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>481</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F189" s="3"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>501</v>
+        <v>529</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="F190" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G190" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>467</v>
+        <v>503</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="F191" s="5" t="s">
-        <v>101</v>
+        <v>504</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -6139,10 +6154,10 @@
         <v>420</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>423</v>
+        <v>501</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>425</v>
+        <v>502</v>
       </c>
       <c r="F192" s="5" t="s">
         <v>101</v>
@@ -6153,10 +6168,10 @@
         <v>420</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F193" s="5" t="s">
         <v>101</v>
@@ -6167,123 +6182,120 @@
         <v>420</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>542</v>
+        <v>423</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="F194" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+      <c r="F194" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>426</v>
+        <v>469</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="F195" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G195" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>470</v>
+      </c>
+      <c r="F195" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>420</v>
       </c>
       <c r="B196" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F197" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C198" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="F196" s="19" t="s">
+      <c r="F198" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="17" t="s">
+    <row r="199" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="B197" s="17" t="s">
+      <c r="B199" s="17" t="s">
         <v>491</v>
       </c>
-      <c r="C197" s="17" t="s">
+      <c r="C199" s="17" t="s">
         <v>492</v>
       </c>
-      <c r="D197" s="17"/>
-      <c r="E197" s="17"/>
-      <c r="F197" s="19" t="s">
+      <c r="D199" s="17"/>
+      <c r="E199" s="17"/>
+      <c r="F199" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G197" s="17"/>
-    </row>
-    <row r="198" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F198" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F199" s="12" t="s">
-        <v>250</v>
-      </c>
+      <c r="G199" s="17"/>
     </row>
     <row r="200" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F200" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>213</v>
+        <v>304</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F201" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G201" s="2" t="s">
-        <v>346</v>
+        <v>305</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F201" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6291,27 +6303,30 @@
         <v>93</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F202" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>94</v>
+        <v>213</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F203" s="5" t="s">
-        <v>101</v>
+        <v>214</v>
+      </c>
+      <c r="F203" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6319,142 +6334,142 @@
         <v>93</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F204" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>218</v>
+        <v>94</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F205" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F205" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B206" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C206" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D206" s="17"/>
-      <c r="E206" s="17"/>
-      <c r="F206" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G206" s="17"/>
+      <c r="B206" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="207" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>71</v>
+        <v>218</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F207" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G207" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F208" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G208" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="F207" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B208" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C208" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D208" s="17"/>
+      <c r="E208" s="17"/>
+      <c r="F208" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G208" s="17"/>
+    </row>
+    <row r="209" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>756</v>
+        <v>71</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>757</v>
+        <v>72</v>
       </c>
       <c r="F209" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F210" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G209" s="2" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B210" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C210" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D210" s="17"/>
-      <c r="E210" s="17"/>
-      <c r="F210" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="G210" s="17" t="s">
-        <v>336</v>
+      <c r="G210" s="2" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>635</v>
+        <v>750</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="F211" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="F212" s="5" t="s">
-        <v>101</v>
+        <v>751</v>
+      </c>
+      <c r="F211" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B212" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C212" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D212" s="17"/>
+      <c r="E212" s="17"/>
+      <c r="F212" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G212" s="17" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6462,10 +6477,10 @@
         <v>73</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>74</v>
+        <v>635</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>82</v>
+        <v>636</v>
       </c>
       <c r="F213" s="4" t="s">
         <v>100</v>
@@ -6476,27 +6491,27 @@
         <v>73</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>75</v>
+        <v>551</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>83</v>
+        <v>552</v>
       </c>
       <c r="F214" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>555</v>
+        <v>74</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="F215" s="5" t="s">
-        <v>101</v>
+        <v>82</v>
+      </c>
+      <c r="F215" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6504,27 +6519,27 @@
         <v>73</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>411</v>
+        <v>75</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="F216" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="F216" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>680</v>
+        <v>555</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="F217" s="4" t="s">
-        <v>100</v>
+        <v>556</v>
+      </c>
+      <c r="F217" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -6532,13 +6547,13 @@
         <v>73</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>553</v>
+        <v>411</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="F218" s="5" t="s">
-        <v>101</v>
+        <v>412</v>
+      </c>
+      <c r="F218" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -6546,69 +6561,69 @@
         <v>73</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>283</v>
+        <v>680</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F219" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="220" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>681</v>
+      </c>
+      <c r="F219" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>256</v>
+        <v>553</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F220" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+      <c r="F220" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>236</v>
+        <v>283</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E221" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F221" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="F221" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>621</v>
+        <v>256</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="F222" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>623</v>
+        <v>236</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>624</v>
+        <v>237</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>101</v>
@@ -6619,10 +6634,10 @@
         <v>73</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>232</v>
+        <v>621</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>233</v>
+        <v>622</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>101</v>
@@ -6633,10 +6648,10 @@
         <v>73</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>228</v>
+        <v>623</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>229</v>
+        <v>624</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>101</v>
@@ -6647,13 +6662,10 @@
         <v>73</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>637</v>
+        <v>232</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="D226" s="2" t="s">
-        <v>639</v>
+        <v>233</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>101</v>
@@ -6664,10 +6676,10 @@
         <v>73</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>625</v>
+        <v>228</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>626</v>
+        <v>229</v>
       </c>
       <c r="F227" s="5" t="s">
         <v>101</v>
@@ -6678,13 +6690,16 @@
         <v>73</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>718</v>
+        <v>637</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="F228" s="3" t="s">
-        <v>99</v>
+        <v>638</v>
+      </c>
+      <c r="D228" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="F228" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -6692,13 +6707,13 @@
         <v>73</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="F229" s="3" t="s">
-        <v>99</v>
+        <v>626</v>
+      </c>
+      <c r="F229" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -6706,10 +6721,10 @@
         <v>73</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>612</v>
+        <v>713</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>613</v>
+        <v>714</v>
       </c>
       <c r="F230" s="3" t="s">
         <v>99</v>
@@ -6720,13 +6735,13 @@
         <v>73</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>590</v>
+        <v>640</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="F231" s="4" t="s">
-        <v>100</v>
+        <v>641</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -6734,30 +6749,27 @@
         <v>73</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>241</v>
+        <v>612</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F232" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>285</v>
+        <v>590</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F233" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="G233" s="2" t="s">
-        <v>334</v>
+        <v>591</v>
+      </c>
+      <c r="F233" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6765,27 +6777,30 @@
         <v>73</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>76</v>
+        <v>241</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F234" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="F234" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>77</v>
+        <v>285</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F235" s="5" t="s">
-        <v>101</v>
+        <v>286</v>
+      </c>
+      <c r="F235" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G235" s="2" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -6793,10 +6808,10 @@
         <v>73</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F236" s="5" t="s">
         <v>101</v>
@@ -6807,27 +6822,24 @@
         <v>73</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F237" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="238" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F237" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>627</v>
+        <v>78</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>629</v>
+        <v>86</v>
       </c>
       <c r="F238" s="5" t="s">
         <v>101</v>
@@ -6838,41 +6850,44 @@
         <v>73</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>448</v>
+        <v>79</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>449</v>
+        <v>87</v>
       </c>
       <c r="F239" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>478</v>
+        <v>627</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F240" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="F240" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>642</v>
+        <v>448</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="F241" s="5" t="s">
-        <v>101</v>
+        <v>449</v>
+      </c>
+      <c r="F241" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -6880,27 +6895,27 @@
         <v>73</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>750</v>
+        <v>478</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>751</v>
-      </c>
-      <c r="F242" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+      <c r="F242" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>80</v>
+        <v>642</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F243" s="3" t="s">
-        <v>99</v>
+        <v>643</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -6908,47 +6923,41 @@
         <v>73</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>549</v>
+        <v>744</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="F244" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>745</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F245" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G245" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>295</v>
+        <v>549</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F246" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G246" s="2" t="s">
-        <v>335</v>
+        <v>550</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="247" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6956,10 +6965,10 @@
         <v>73</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>240</v>
+        <v>294</v>
       </c>
       <c r="F247" s="16" t="s">
         <v>303</v>
@@ -6968,80 +6977,83 @@
         <v>335</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>230</v>
+        <v>295</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E248" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F248" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="F248" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G248" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>698</v>
+        <v>239</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>699</v>
-      </c>
-      <c r="F249" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="F249" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G249" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>81</v>
+        <v>230</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>89</v>
+        <v>231</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F250" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>754</v>
+        <v>696</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="F251" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>697</v>
+      </c>
+      <c r="F251" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>443</v>
+        <v>81</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F252" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G252" s="2" t="s">
-        <v>377</v>
+        <v>89</v>
+      </c>
+      <c r="F252" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -7049,27 +7061,30 @@
         <v>73</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>644</v>
+        <v>748</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="F253" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+        <v>749</v>
+      </c>
+      <c r="F253" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>507</v>
+        <v>443</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="F254" s="5" t="s">
-        <v>101</v>
+        <v>444</v>
+      </c>
+      <c r="F254" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G254" s="2" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -7077,13 +7092,13 @@
         <v>73</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>245</v>
+        <v>644</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F255" s="14" t="s">
-        <v>258</v>
+        <v>645</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -7091,10 +7106,10 @@
         <v>73</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>298</v>
+        <v>507</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>297</v>
+        <v>508</v>
       </c>
       <c r="F256" s="5" t="s">
         <v>101</v>
@@ -7105,13 +7120,13 @@
         <v>73</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>646</v>
+        <v>245</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="F257" s="4" t="s">
-        <v>100</v>
+        <v>246</v>
+      </c>
+      <c r="F257" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -7119,10 +7134,10 @@
         <v>73</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>234</v>
+        <v>298</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>235</v>
+        <v>297</v>
       </c>
       <c r="F258" s="5" t="s">
         <v>101</v>
@@ -7133,13 +7148,13 @@
         <v>73</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>630</v>
+        <v>646</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="F259" s="5" t="s">
-        <v>101</v>
+        <v>647</v>
+      </c>
+      <c r="F259" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -7147,13 +7162,13 @@
         <v>73</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F260" s="12" t="s">
-        <v>250</v>
+        <v>235</v>
+      </c>
+      <c r="F260" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -7161,13 +7176,13 @@
         <v>73</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>524</v>
+        <v>630</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F261" s="14" t="s">
-        <v>258</v>
+        <v>631</v>
+      </c>
+      <c r="F261" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -7175,16 +7190,13 @@
         <v>73</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>522</v>
+        <v>226</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E262" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F262" s="5" t="s">
-        <v>101</v>
+        <v>227</v>
+      </c>
+      <c r="F262" s="12" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -7192,126 +7204,123 @@
         <v>73</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>224</v>
+        <v>524</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F263" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="264" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>525</v>
+      </c>
+      <c r="F263" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>648</v>
+        <v>522</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="F264" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="265" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+      <c r="E264" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F264" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>585</v>
+        <v>224</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="F265" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G265" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="F265" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>586</v>
+        <v>648</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="F266" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G266" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="267" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="F266" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B267" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="C267" s="17" t="s">
-        <v>307</v>
-      </c>
-      <c r="D267" s="17"/>
-      <c r="E267" s="17"/>
-      <c r="F267" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G267" s="17"/>
+      <c r="B267" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F267" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G267" s="2" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="268" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>91</v>
+        <v>586</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D268" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F268" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B269" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D269" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="F269" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="270" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>589</v>
+      </c>
+      <c r="F268" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G268" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B269" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="C269" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="D269" s="17"/>
+      <c r="E269" s="17"/>
+      <c r="F269" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G269" s="17"/>
+    </row>
+    <row r="270" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>247</v>
+        <v>91</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>248</v>
+        <v>92</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>249</v>
+        <v>315</v>
       </c>
       <c r="F270" s="5" t="s">
         <v>101</v>
@@ -7322,50 +7331,84 @@
         <v>90</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>351</v>
+        <v>222</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F271" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+      <c r="D271" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="F271" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B272" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D272" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F272" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F273" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B274" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="C272" s="2" t="s">
+      <c r="C274" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="D272" s="2" t="s">
+      <c r="D274" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="F272" s="4" t="s">
+      <c r="F274" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="273" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="17" t="s">
+    <row r="275" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B273" s="17" t="s">
+      <c r="B275" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="C273" s="17" t="s">
+      <c r="C275" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="D273" s="17" t="s">
+      <c r="D275" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="E273" s="17"/>
-      <c r="F273" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G273" s="17"/>
+      <c r="E275" s="17"/>
+      <c r="F275" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G275" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>